<commit_message>
Caso de uso - cadastro colaborador
</commit_message>
<xml_diff>
--- a/testes/cmproject_test_case.xlsx
+++ b/testes/cmproject_test_case.xlsx
@@ -17,14 +17,15 @@
     <sheet name="UC - Alugar Veículo" sheetId="3" r:id="rId3"/>
     <sheet name="UC - Login" sheetId="4" r:id="rId4"/>
     <sheet name="UC - Cadastro Visitante" sheetId="5" r:id="rId5"/>
-    <sheet name="UC - Consultar veículos" sheetId="6" r:id="rId6"/>
+    <sheet name="UC - Cadastro Colaborador" sheetId="7" r:id="rId6"/>
+    <sheet name="UC - Consultar veículos" sheetId="6" r:id="rId7"/>
   </sheets>
   <calcPr calcId="0" iterateDelta="1E-4"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="143">
   <si>
     <t>Projeto de Teste</t>
   </si>
@@ -421,6 +422,42 @@
   </si>
   <si>
     <t>SABER SE A FUNÇÃO CADASTRO DE VISITANTES ESTÁ FUNCIONANDO CORRETAMENTE</t>
+  </si>
+  <si>
+    <t>Cadastro Visitante</t>
+  </si>
+  <si>
+    <t>Cadastro Colaborador</t>
+  </si>
+  <si>
+    <t>SABER SE A FUNÇÃO CADASTRO DE COLABORADORES ESTÁ FUNCIONANDO CORRETAMENTE</t>
+  </si>
+  <si>
+    <t>Cadastrar Colaboradores</t>
+  </si>
+  <si>
+    <t>Cadastrar colaborador, e depois cadastrar novo colaborador com o mesmo email.</t>
+  </si>
+  <si>
+    <t>Ter colaborador com o mesmo email que vai ser cadastrado já previamente cadastrado</t>
+  </si>
+  <si>
+    <t>Cadastrar colaborador com o mesmo email</t>
+  </si>
+  <si>
+    <t>Cadastrar colaborador com o mesmo cpf</t>
+  </si>
+  <si>
+    <t>Ter colaborador com o mesmo cpf que vai ser cadastrado já previamente cadastrado</t>
+  </si>
+  <si>
+    <t>Cadastrar colaborador e depois cadastrar novo usuário com o mesmo cpf.</t>
+  </si>
+  <si>
+    <t>Cadastrar colaborador sem preencher os campos do formulário</t>
+  </si>
+  <si>
+    <t>Clicar no botão CADASTRAR da tela de cadastro de colaboradores sem preencher os campos solicitados</t>
   </si>
 </sst>
 </file>
@@ -1771,7 +1808,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G76"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
@@ -2538,7 +2575,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G48"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
@@ -3101,7 +3138,7 @@
   <dimension ref="A1:G59"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:D3"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3141,7 +3178,7 @@
         <v>9</v>
       </c>
       <c r="B2" s="32" t="s">
-        <v>58</v>
+        <v>131</v>
       </c>
       <c r="C2" s="33"/>
       <c r="D2" s="34"/>
@@ -3703,10 +3740,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G57"/>
+  <dimension ref="A1:G59"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:D3"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3746,7 +3783,7 @@
         <v>9</v>
       </c>
       <c r="B2" s="32" t="s">
-        <v>58</v>
+        <v>132</v>
       </c>
       <c r="C2" s="33"/>
       <c r="D2" s="34"/>
@@ -3761,7 +3798,7 @@
         <v>11</v>
       </c>
       <c r="B3" s="81" t="s">
-        <v>129</v>
+        <v>133</v>
       </c>
       <c r="C3" s="81"/>
       <c r="D3" s="81"/>
@@ -3799,25 +3836,25 @@
     </row>
     <row r="6" spans="1:7" ht="97.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="48" t="s">
-        <v>123</v>
+        <v>101</v>
       </c>
       <c r="B6" s="49" t="s">
-        <v>124</v>
+        <v>134</v>
       </c>
       <c r="C6" s="49" t="s">
-        <v>125</v>
+        <v>103</v>
       </c>
       <c r="D6" s="49" t="s">
-        <v>126</v>
+        <v>104</v>
       </c>
       <c r="E6" s="50" t="s">
-        <v>127</v>
+        <v>105</v>
       </c>
       <c r="F6" s="51" t="s">
-        <v>128</v>
+        <v>106</v>
       </c>
       <c r="G6" s="75" t="s">
-        <v>127</v>
+        <v>107</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
@@ -3830,13 +3867,27 @@
       <c r="G7" s="76"/>
     </row>
     <row r="8" spans="1:7" ht="97.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="48"/>
-      <c r="B8" s="49"/>
-      <c r="C8" s="49"/>
-      <c r="D8" s="49"/>
-      <c r="E8" s="50"/>
-      <c r="F8" s="51"/>
-      <c r="G8" s="78"/>
+      <c r="A8" s="48" t="s">
+        <v>108</v>
+      </c>
+      <c r="B8" s="49" t="s">
+        <v>137</v>
+      </c>
+      <c r="C8" s="49" t="s">
+        <v>136</v>
+      </c>
+      <c r="D8" s="49" t="s">
+        <v>135</v>
+      </c>
+      <c r="E8" s="50" t="s">
+        <v>112</v>
+      </c>
+      <c r="F8" s="51" t="s">
+        <v>106</v>
+      </c>
+      <c r="G8" s="77" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" s="53"/>
@@ -3848,13 +3899,27 @@
       <c r="G9" s="76"/>
     </row>
     <row r="10" spans="1:7" ht="72.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="48"/>
-      <c r="B10" s="49"/>
-      <c r="C10" s="49"/>
-      <c r="D10" s="49"/>
-      <c r="E10" s="50"/>
-      <c r="F10" s="51"/>
-      <c r="G10" s="78"/>
+      <c r="A10" s="48" t="s">
+        <v>114</v>
+      </c>
+      <c r="B10" s="49" t="s">
+        <v>138</v>
+      </c>
+      <c r="C10" s="49" t="s">
+        <v>139</v>
+      </c>
+      <c r="D10" s="49" t="s">
+        <v>140</v>
+      </c>
+      <c r="E10" s="50" t="s">
+        <v>113</v>
+      </c>
+      <c r="F10" s="51" t="s">
+        <v>106</v>
+      </c>
+      <c r="G10" s="75" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" s="53"/>
@@ -3865,6 +3930,582 @@
       <c r="F11" s="54"/>
       <c r="G11" s="76"/>
     </row>
+    <row r="12" spans="1:7" ht="63.75" x14ac:dyDescent="0.2">
+      <c r="A12" s="48" t="s">
+        <v>118</v>
+      </c>
+      <c r="B12" s="49" t="s">
+        <v>141</v>
+      </c>
+      <c r="C12" s="49" t="s">
+        <v>103</v>
+      </c>
+      <c r="D12" s="49" t="s">
+        <v>142</v>
+      </c>
+      <c r="E12" s="50" t="s">
+        <v>122</v>
+      </c>
+      <c r="F12" s="51" t="s">
+        <v>121</v>
+      </c>
+      <c r="G12" s="75" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A13" s="53"/>
+      <c r="B13" s="54"/>
+      <c r="C13" s="54"/>
+      <c r="D13" s="54"/>
+      <c r="E13" s="54"/>
+      <c r="F13" s="54"/>
+      <c r="G13" s="76"/>
+    </row>
+    <row r="14" spans="1:7" ht="60" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="48"/>
+      <c r="B14" s="49"/>
+      <c r="C14" s="49"/>
+      <c r="D14" s="49"/>
+      <c r="E14" s="50"/>
+      <c r="F14" s="51"/>
+      <c r="G14" s="78"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A15" s="53"/>
+      <c r="B15" s="54"/>
+      <c r="C15" s="54"/>
+      <c r="D15" s="54"/>
+      <c r="E15" s="54"/>
+      <c r="F15" s="54"/>
+      <c r="G15" s="76"/>
+    </row>
+    <row r="16" spans="1:7" ht="56.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="48"/>
+      <c r="B16" s="49"/>
+      <c r="C16" s="49"/>
+      <c r="D16" s="49"/>
+      <c r="E16" s="50"/>
+      <c r="F16" s="56"/>
+      <c r="G16" s="78"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A17" s="53"/>
+      <c r="B17" s="54"/>
+      <c r="C17" s="54"/>
+      <c r="D17" s="54"/>
+      <c r="E17" s="54"/>
+      <c r="F17" s="54"/>
+      <c r="G17" s="76"/>
+    </row>
+    <row r="18" spans="1:7" ht="47.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="48"/>
+      <c r="B18" s="49"/>
+      <c r="C18" s="49"/>
+      <c r="D18" s="49"/>
+      <c r="E18" s="50"/>
+      <c r="F18" s="56"/>
+      <c r="G18" s="78"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A19" s="57"/>
+      <c r="B19" s="54"/>
+      <c r="C19" s="54"/>
+      <c r="D19" s="54"/>
+      <c r="E19" s="54"/>
+      <c r="F19" s="54"/>
+      <c r="G19" s="76"/>
+    </row>
+    <row r="20" spans="1:7" ht="54" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="48"/>
+      <c r="B20" s="58"/>
+      <c r="C20" s="58"/>
+      <c r="D20" s="58"/>
+      <c r="E20" s="59"/>
+      <c r="F20" s="60"/>
+      <c r="G20" s="78"/>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A21" s="62"/>
+      <c r="B21" s="63"/>
+      <c r="C21" s="54"/>
+      <c r="D21" s="54"/>
+      <c r="E21" s="54"/>
+      <c r="F21" s="54"/>
+      <c r="G21" s="76"/>
+    </row>
+    <row r="22" spans="1:7" ht="56.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="48"/>
+      <c r="B22" s="58"/>
+      <c r="C22" s="58"/>
+      <c r="D22" s="58"/>
+      <c r="E22" s="59"/>
+      <c r="F22" s="60"/>
+      <c r="G22" s="78"/>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A23" s="64"/>
+      <c r="B23" s="63"/>
+      <c r="C23" s="54"/>
+      <c r="D23" s="54"/>
+      <c r="E23" s="54"/>
+      <c r="F23" s="54"/>
+      <c r="G23" s="76"/>
+    </row>
+    <row r="24" spans="1:7" ht="62.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="48"/>
+      <c r="B24" s="58"/>
+      <c r="C24" s="58"/>
+      <c r="D24" s="58"/>
+      <c r="E24" s="59"/>
+      <c r="F24" s="60"/>
+      <c r="G24" s="78"/>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A25" s="64"/>
+      <c r="B25" s="63"/>
+      <c r="C25" s="54"/>
+      <c r="D25" s="54"/>
+      <c r="E25" s="54"/>
+      <c r="F25" s="54"/>
+      <c r="G25" s="76"/>
+    </row>
+    <row r="26" spans="1:7" ht="56.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="48"/>
+      <c r="B26" s="58"/>
+      <c r="C26" s="58"/>
+      <c r="D26" s="58"/>
+      <c r="E26" s="59"/>
+      <c r="F26" s="60"/>
+      <c r="G26" s="78"/>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A27" s="57"/>
+      <c r="B27" s="55"/>
+      <c r="C27" s="54"/>
+      <c r="D27" s="54"/>
+      <c r="E27" s="54"/>
+      <c r="F27" s="54"/>
+      <c r="G27" s="76"/>
+    </row>
+    <row r="28" spans="1:7" ht="65.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="48"/>
+      <c r="B28" s="58"/>
+      <c r="C28" s="58"/>
+      <c r="D28" s="58"/>
+      <c r="E28" s="59"/>
+      <c r="F28" s="60"/>
+      <c r="G28" s="78"/>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A29" s="57"/>
+      <c r="B29" s="54"/>
+      <c r="C29" s="54"/>
+      <c r="D29" s="54"/>
+      <c r="E29" s="54"/>
+      <c r="F29" s="54"/>
+      <c r="G29" s="76"/>
+    </row>
+    <row r="30" spans="1:7" ht="58.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="48"/>
+      <c r="B30" s="49"/>
+      <c r="C30" s="49"/>
+      <c r="D30" s="58"/>
+      <c r="E30" s="50"/>
+      <c r="F30" s="60"/>
+      <c r="G30" s="78"/>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A31" s="53"/>
+      <c r="B31" s="54"/>
+      <c r="C31" s="54"/>
+      <c r="D31" s="54"/>
+      <c r="E31" s="54"/>
+      <c r="F31" s="54"/>
+      <c r="G31" s="76"/>
+    </row>
+    <row r="32" spans="1:7" ht="56.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="48"/>
+      <c r="B32" s="49"/>
+      <c r="C32" s="58"/>
+      <c r="D32" s="58"/>
+      <c r="E32" s="59"/>
+      <c r="F32" s="60"/>
+      <c r="G32" s="78"/>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A33" s="53"/>
+      <c r="B33" s="54"/>
+      <c r="C33" s="54"/>
+      <c r="D33" s="54"/>
+      <c r="E33" s="54"/>
+      <c r="F33" s="54"/>
+      <c r="G33" s="76"/>
+    </row>
+    <row r="34" spans="1:7" ht="69" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="48"/>
+      <c r="B34" s="49"/>
+      <c r="C34" s="49"/>
+      <c r="D34" s="58"/>
+      <c r="E34" s="50"/>
+      <c r="F34" s="51"/>
+      <c r="G34" s="78"/>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A35" s="53"/>
+      <c r="B35" s="54"/>
+      <c r="C35" s="54"/>
+      <c r="D35" s="54"/>
+      <c r="E35" s="54"/>
+      <c r="F35" s="54"/>
+      <c r="G35" s="76"/>
+    </row>
+    <row r="36" spans="1:7" ht="58.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A36" s="48"/>
+      <c r="B36" s="49"/>
+      <c r="C36" s="49"/>
+      <c r="D36" s="58"/>
+      <c r="E36" s="50"/>
+      <c r="F36" s="51"/>
+      <c r="G36" s="78"/>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A37" s="53"/>
+      <c r="B37" s="54"/>
+      <c r="C37" s="54"/>
+      <c r="D37" s="54"/>
+      <c r="E37" s="54"/>
+      <c r="F37" s="54"/>
+      <c r="G37" s="76"/>
+    </row>
+    <row r="38" spans="1:7" ht="54" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A38" s="48"/>
+      <c r="B38" s="49"/>
+      <c r="C38" s="49"/>
+      <c r="D38" s="58"/>
+      <c r="E38" s="50"/>
+      <c r="F38" s="51"/>
+      <c r="G38" s="78"/>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A39" s="53"/>
+      <c r="B39" s="54"/>
+      <c r="C39" s="54"/>
+      <c r="D39" s="54"/>
+      <c r="E39" s="54"/>
+      <c r="F39" s="54"/>
+      <c r="G39" s="76"/>
+    </row>
+    <row r="40" spans="1:7" ht="63.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A40" s="48"/>
+      <c r="B40" s="49"/>
+      <c r="C40" s="49"/>
+      <c r="D40" s="58"/>
+      <c r="E40" s="50"/>
+      <c r="F40" s="51"/>
+      <c r="G40" s="78"/>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A41" s="53"/>
+      <c r="B41" s="54"/>
+      <c r="C41" s="54"/>
+      <c r="D41" s="54"/>
+      <c r="E41" s="54"/>
+      <c r="F41" s="54"/>
+      <c r="G41" s="76"/>
+    </row>
+    <row r="42" spans="1:7" ht="61.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A42" s="48"/>
+      <c r="B42" s="49"/>
+      <c r="C42" s="49"/>
+      <c r="D42" s="58"/>
+      <c r="E42" s="50"/>
+      <c r="F42" s="51"/>
+      <c r="G42" s="78"/>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A43" s="65"/>
+      <c r="B43" s="66"/>
+      <c r="C43" s="66"/>
+      <c r="D43" s="66"/>
+      <c r="E43" s="66"/>
+      <c r="F43" s="66"/>
+      <c r="G43" s="79"/>
+    </row>
+    <row r="44" spans="1:7" ht="64.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A44" s="48"/>
+      <c r="B44" s="49"/>
+      <c r="C44" s="49"/>
+      <c r="D44" s="58"/>
+      <c r="E44" s="50"/>
+      <c r="F44" s="51"/>
+      <c r="G44" s="78"/>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A45" s="65"/>
+      <c r="B45" s="66"/>
+      <c r="C45" s="66"/>
+      <c r="D45" s="66"/>
+      <c r="E45" s="66"/>
+      <c r="F45" s="66"/>
+      <c r="G45" s="79"/>
+    </row>
+    <row r="46" spans="1:7" ht="57.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A46" s="48"/>
+      <c r="B46" s="58"/>
+      <c r="C46" s="58"/>
+      <c r="D46" s="58"/>
+      <c r="E46" s="59"/>
+      <c r="F46" s="60"/>
+      <c r="G46" s="78"/>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A47" s="65"/>
+    </row>
+    <row r="48" spans="1:7" ht="60" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A48" s="48"/>
+      <c r="B48" s="58"/>
+      <c r="C48" s="58"/>
+      <c r="D48" s="58"/>
+      <c r="E48" s="59"/>
+      <c r="F48" s="60"/>
+      <c r="G48" s="78"/>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A49" s="65"/>
+    </row>
+    <row r="50" spans="1:7" ht="58.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A50" s="48"/>
+      <c r="B50" s="58"/>
+      <c r="C50" s="58"/>
+      <c r="D50" s="58"/>
+      <c r="E50" s="59"/>
+      <c r="F50" s="60"/>
+      <c r="G50" s="78"/>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A51" s="65"/>
+    </row>
+    <row r="52" spans="1:7" ht="55.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A52" s="48"/>
+      <c r="B52" s="58"/>
+      <c r="C52" s="58"/>
+      <c r="D52" s="58"/>
+      <c r="E52" s="59"/>
+      <c r="F52" s="60"/>
+      <c r="G52" s="78"/>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A53" s="65"/>
+    </row>
+    <row r="54" spans="1:7" ht="55.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A54" s="48"/>
+      <c r="B54" s="49"/>
+      <c r="C54" s="49"/>
+      <c r="D54" s="49"/>
+      <c r="E54" s="50"/>
+      <c r="F54" s="51"/>
+      <c r="G54" s="78"/>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A55" s="65"/>
+    </row>
+    <row r="56" spans="1:7" ht="51.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A56" s="48"/>
+      <c r="B56" s="49"/>
+      <c r="C56" s="49"/>
+      <c r="D56" s="49"/>
+      <c r="E56" s="50"/>
+      <c r="F56" s="51"/>
+      <c r="G56" s="78"/>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A57" s="65"/>
+    </row>
+    <row r="58" spans="1:7" ht="52.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A58" s="48"/>
+      <c r="B58" s="49"/>
+      <c r="C58" s="49"/>
+      <c r="D58" s="49"/>
+      <c r="E58" s="50"/>
+      <c r="F58" s="51"/>
+      <c r="G58" s="78"/>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A59" s="65"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B3:D3"/>
+  </mergeCells>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G57"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="17" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="28.42578125" customWidth="1"/>
+    <col min="5" max="5" width="33.42578125" customWidth="1"/>
+    <col min="6" max="6" width="25.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="26.7109375" style="80" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="25" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="26" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="27"/>
+      <c r="D1" s="28" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" s="29" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="30" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" s="31" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="32" t="s">
+        <v>58</v>
+      </c>
+      <c r="C2" s="33"/>
+      <c r="D2" s="34"/>
+      <c r="E2" s="35" t="s">
+        <v>59</v>
+      </c>
+      <c r="F2" s="36"/>
+      <c r="G2" s="73"/>
+    </row>
+    <row r="3" spans="1:7" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="25" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="81" t="s">
+        <v>129</v>
+      </c>
+      <c r="C3" s="81"/>
+      <c r="D3" s="81"/>
+      <c r="E3" s="38"/>
+      <c r="F3" s="39"/>
+      <c r="G3" s="73"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E4" s="40"/>
+      <c r="F4" s="41"/>
+      <c r="G4" s="74"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" s="43" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="44" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="43" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" s="43" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5" s="45" t="s">
+        <v>17</v>
+      </c>
+      <c r="F5" s="46" t="s">
+        <v>18</v>
+      </c>
+      <c r="G5" s="47" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="97.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="48" t="s">
+        <v>123</v>
+      </c>
+      <c r="B6" s="49" t="s">
+        <v>124</v>
+      </c>
+      <c r="C6" s="49" t="s">
+        <v>125</v>
+      </c>
+      <c r="D6" s="49" t="s">
+        <v>126</v>
+      </c>
+      <c r="E6" s="50" t="s">
+        <v>127</v>
+      </c>
+      <c r="F6" s="51" t="s">
+        <v>128</v>
+      </c>
+      <c r="G6" s="75" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7" s="53"/>
+      <c r="B7" s="54"/>
+      <c r="C7" s="54"/>
+      <c r="D7" s="54"/>
+      <c r="E7" s="54"/>
+      <c r="F7" s="54"/>
+      <c r="G7" s="76"/>
+    </row>
+    <row r="8" spans="1:7" ht="97.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="48"/>
+      <c r="B8" s="49"/>
+      <c r="C8" s="49"/>
+      <c r="D8" s="49"/>
+      <c r="E8" s="50"/>
+      <c r="F8" s="51"/>
+      <c r="G8" s="78"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9" s="53"/>
+      <c r="B9" s="54"/>
+      <c r="C9" s="54"/>
+      <c r="D9" s="54"/>
+      <c r="E9" s="54"/>
+      <c r="F9" s="54"/>
+      <c r="G9" s="76"/>
+    </row>
+    <row r="10" spans="1:7" ht="72.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="48"/>
+      <c r="B10" s="49"/>
+      <c r="C10" s="49"/>
+      <c r="D10" s="49"/>
+      <c r="E10" s="50"/>
+      <c r="F10" s="51"/>
+      <c r="G10" s="78"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11" s="53"/>
+      <c r="B11" s="55"/>
+      <c r="C11" s="54"/>
+      <c r="D11" s="54"/>
+      <c r="E11" s="54"/>
+      <c r="F11" s="54"/>
+      <c r="G11" s="76"/>
+    </row>
     <row r="12" spans="1:7" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="48"/>
       <c r="B12" s="49"/>

</xml_diff>

<commit_message>
Caso de teste - Consultar veículos
</commit_message>
<xml_diff>
--- a/testes/cmproject_test_case.xlsx
+++ b/testes/cmproject_test_case.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="990" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="856" firstSheet="2" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Capa" sheetId="1" r:id="rId1"/>
@@ -18,14 +18,15 @@
     <sheet name="UC - Login" sheetId="4" r:id="rId4"/>
     <sheet name="UC - Cadastro Visitante" sheetId="5" r:id="rId5"/>
     <sheet name="UC - Cadastro Colaborador" sheetId="7" r:id="rId6"/>
-    <sheet name="UC - Consultar veículos" sheetId="6" r:id="rId7"/>
+    <sheet name="UC - Cadastrar Veículos" sheetId="8" r:id="rId7"/>
+    <sheet name="UC - Consultar veículos" sheetId="6" r:id="rId8"/>
   </sheets>
   <calcPr calcId="0" iterateDelta="1E-4"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="164">
   <si>
     <t>Projeto de Teste</t>
   </si>
@@ -458,6 +459,69 @@
   </si>
   <si>
     <t>Clicar no botão CADASTRAR da tela de cadastro de colaboradores sem preencher os campos solicitados</t>
+  </si>
+  <si>
+    <t>Cadastrar Veículos</t>
+  </si>
+  <si>
+    <t>CT-e001</t>
+  </si>
+  <si>
+    <t>Cadastrar veículo</t>
+  </si>
+  <si>
+    <t>REALIZAR LOGIN, ACESSAR AÇÕES ADMINISTRATIVAS, CLICAR EM CADASTRO DE VEÍCULO, PREENCHER OS CAMPOS SOLICITADOS</t>
+  </si>
+  <si>
+    <t>TER CADASTRO NO SISTEMA</t>
+  </si>
+  <si>
+    <t>dados solicitados no formulário</t>
+  </si>
+  <si>
+    <t>CT-e002</t>
+  </si>
+  <si>
+    <t>Cadastro de veículo com campos incompletos</t>
+  </si>
+  <si>
+    <t>REALIZAR LOGIN, ACESSAR AÇÕES ADMINISTRATIVAS, CLICAR EM CADASTRO DE VEÍCULO, PREENCHER ALGUNS DOS CAMPOS SOLICITADOS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MENSAGEM SOLICITANTO O PREENCHIMENTO DOS CAMPOS FALTANTES </t>
+  </si>
+  <si>
+    <t>CT-e003</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cadastro de imagem de veículo </t>
+  </si>
+  <si>
+    <t>IMAGEM SALVA NO SERVIDOR E VISÍVEL NA LISTA DE NOSSOS VEÍCULOS</t>
+  </si>
+  <si>
+    <t>ARQUIVO DE IMAGEM NO CAMPO DO FORMULÁRIO</t>
+  </si>
+  <si>
+    <t>IMAGEM NÃO SALVA E NEM SENDO EXIBIDA NA LISTA DE NOSSOS VEÍCULOS.</t>
+  </si>
+  <si>
+    <t>CT-e004</t>
+  </si>
+  <si>
+    <t>CT-d002</t>
+  </si>
+  <si>
+    <t>Exibir imagens dos veículos na lista</t>
+  </si>
+  <si>
+    <t>LISTA COM TODOS OS VEÍCULOS CADASTRADOS COM AS RESPECTIVAS IMAGENS</t>
+  </si>
+  <si>
+    <t>CAMPO IMAGEM NÃO RETORNA IMAGEM DO VEÍCULO</t>
+  </si>
+  <si>
+    <t>Concultar veículos</t>
   </si>
 </sst>
 </file>
@@ -3742,8 +3806,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C8" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4346,8 +4410,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G57"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4387,7 +4451,7 @@
         <v>9</v>
       </c>
       <c r="B2" s="32" t="s">
-        <v>58</v>
+        <v>143</v>
       </c>
       <c r="C2" s="33"/>
       <c r="D2" s="34"/>
@@ -4402,7 +4466,7 @@
         <v>11</v>
       </c>
       <c r="B3" s="81" t="s">
-        <v>129</v>
+        <v>133</v>
       </c>
       <c r="C3" s="81"/>
       <c r="D3" s="81"/>
@@ -4440,25 +4504,25 @@
     </row>
     <row r="6" spans="1:7" ht="97.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="48" t="s">
-        <v>123</v>
+        <v>144</v>
       </c>
       <c r="B6" s="49" t="s">
-        <v>124</v>
+        <v>145</v>
       </c>
       <c r="C6" s="49" t="s">
-        <v>125</v>
+        <v>147</v>
       </c>
       <c r="D6" s="49" t="s">
-        <v>126</v>
+        <v>146</v>
       </c>
       <c r="E6" s="50" t="s">
-        <v>127</v>
+        <v>107</v>
       </c>
       <c r="F6" s="51" t="s">
-        <v>128</v>
+        <v>148</v>
       </c>
       <c r="G6" s="75" t="s">
-        <v>127</v>
+        <v>107</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
@@ -4471,13 +4535,27 @@
       <c r="G7" s="76"/>
     </row>
     <row r="8" spans="1:7" ht="97.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="48"/>
-      <c r="B8" s="49"/>
-      <c r="C8" s="49"/>
-      <c r="D8" s="49"/>
-      <c r="E8" s="50"/>
-      <c r="F8" s="51"/>
-      <c r="G8" s="78"/>
+      <c r="A8" s="48" t="s">
+        <v>149</v>
+      </c>
+      <c r="B8" s="49" t="s">
+        <v>150</v>
+      </c>
+      <c r="C8" s="49" t="s">
+        <v>147</v>
+      </c>
+      <c r="D8" s="49" t="s">
+        <v>151</v>
+      </c>
+      <c r="E8" s="50" t="s">
+        <v>152</v>
+      </c>
+      <c r="F8" s="51" t="s">
+        <v>148</v>
+      </c>
+      <c r="G8" s="75" t="s">
+        <v>152</v>
+      </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" s="53"/>
@@ -4489,6 +4567,580 @@
       <c r="G9" s="76"/>
     </row>
     <row r="10" spans="1:7" ht="72.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="48" t="s">
+        <v>153</v>
+      </c>
+      <c r="B10" s="49" t="s">
+        <v>154</v>
+      </c>
+      <c r="C10" s="49" t="s">
+        <v>147</v>
+      </c>
+      <c r="D10" s="49" t="s">
+        <v>146</v>
+      </c>
+      <c r="E10" s="50" t="s">
+        <v>155</v>
+      </c>
+      <c r="F10" s="51" t="s">
+        <v>156</v>
+      </c>
+      <c r="G10" s="77" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11" s="53"/>
+      <c r="B11" s="54"/>
+      <c r="C11" s="54"/>
+      <c r="D11" s="54"/>
+      <c r="E11" s="54"/>
+      <c r="F11" s="54"/>
+      <c r="G11" s="76"/>
+    </row>
+    <row r="12" spans="1:7" ht="60" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="48" t="s">
+        <v>158</v>
+      </c>
+      <c r="B12" s="49"/>
+      <c r="C12" s="49"/>
+      <c r="D12" s="49"/>
+      <c r="E12" s="50"/>
+      <c r="F12" s="51"/>
+      <c r="G12" s="78"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A13" s="53"/>
+      <c r="B13" s="54"/>
+      <c r="C13" s="54"/>
+      <c r="D13" s="54"/>
+      <c r="E13" s="54"/>
+      <c r="F13" s="54"/>
+      <c r="G13" s="76"/>
+    </row>
+    <row r="14" spans="1:7" ht="56.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="48"/>
+      <c r="B14" s="49"/>
+      <c r="C14" s="49"/>
+      <c r="D14" s="49"/>
+      <c r="E14" s="50"/>
+      <c r="F14" s="56"/>
+      <c r="G14" s="78"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A15" s="53"/>
+      <c r="B15" s="54"/>
+      <c r="C15" s="54"/>
+      <c r="D15" s="54"/>
+      <c r="E15" s="54"/>
+      <c r="F15" s="54"/>
+      <c r="G15" s="76"/>
+    </row>
+    <row r="16" spans="1:7" ht="47.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="48"/>
+      <c r="B16" s="49"/>
+      <c r="C16" s="49"/>
+      <c r="D16" s="49"/>
+      <c r="E16" s="50"/>
+      <c r="F16" s="56"/>
+      <c r="G16" s="78"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A17" s="57"/>
+      <c r="B17" s="54"/>
+      <c r="C17" s="54"/>
+      <c r="D17" s="54"/>
+      <c r="E17" s="54"/>
+      <c r="F17" s="54"/>
+      <c r="G17" s="76"/>
+    </row>
+    <row r="18" spans="1:7" ht="54" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="48"/>
+      <c r="B18" s="58"/>
+      <c r="C18" s="58"/>
+      <c r="D18" s="58"/>
+      <c r="E18" s="59"/>
+      <c r="F18" s="60"/>
+      <c r="G18" s="78"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A19" s="62"/>
+      <c r="B19" s="63"/>
+      <c r="C19" s="54"/>
+      <c r="D19" s="54"/>
+      <c r="E19" s="54"/>
+      <c r="F19" s="54"/>
+      <c r="G19" s="76"/>
+    </row>
+    <row r="20" spans="1:7" ht="56.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="48"/>
+      <c r="B20" s="58"/>
+      <c r="C20" s="58"/>
+      <c r="D20" s="58"/>
+      <c r="E20" s="59"/>
+      <c r="F20" s="60"/>
+      <c r="G20" s="78"/>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A21" s="64"/>
+      <c r="B21" s="63"/>
+      <c r="C21" s="54"/>
+      <c r="D21" s="54"/>
+      <c r="E21" s="54"/>
+      <c r="F21" s="54"/>
+      <c r="G21" s="76"/>
+    </row>
+    <row r="22" spans="1:7" ht="62.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="48"/>
+      <c r="B22" s="58"/>
+      <c r="C22" s="58"/>
+      <c r="D22" s="58"/>
+      <c r="E22" s="59"/>
+      <c r="F22" s="60"/>
+      <c r="G22" s="78"/>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A23" s="64"/>
+      <c r="B23" s="63"/>
+      <c r="C23" s="54"/>
+      <c r="D23" s="54"/>
+      <c r="E23" s="54"/>
+      <c r="F23" s="54"/>
+      <c r="G23" s="76"/>
+    </row>
+    <row r="24" spans="1:7" ht="56.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="48"/>
+      <c r="B24" s="58"/>
+      <c r="C24" s="58"/>
+      <c r="D24" s="58"/>
+      <c r="E24" s="59"/>
+      <c r="F24" s="60"/>
+      <c r="G24" s="78"/>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A25" s="57"/>
+      <c r="B25" s="55"/>
+      <c r="C25" s="54"/>
+      <c r="D25" s="54"/>
+      <c r="E25" s="54"/>
+      <c r="F25" s="54"/>
+      <c r="G25" s="76"/>
+    </row>
+    <row r="26" spans="1:7" ht="65.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="48"/>
+      <c r="B26" s="58"/>
+      <c r="C26" s="58"/>
+      <c r="D26" s="58"/>
+      <c r="E26" s="59"/>
+      <c r="F26" s="60"/>
+      <c r="G26" s="78"/>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A27" s="57"/>
+      <c r="B27" s="54"/>
+      <c r="C27" s="54"/>
+      <c r="D27" s="54"/>
+      <c r="E27" s="54"/>
+      <c r="F27" s="54"/>
+      <c r="G27" s="76"/>
+    </row>
+    <row r="28" spans="1:7" ht="58.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="48"/>
+      <c r="B28" s="49"/>
+      <c r="C28" s="49"/>
+      <c r="D28" s="58"/>
+      <c r="E28" s="50"/>
+      <c r="F28" s="60"/>
+      <c r="G28" s="78"/>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A29" s="53"/>
+      <c r="B29" s="54"/>
+      <c r="C29" s="54"/>
+      <c r="D29" s="54"/>
+      <c r="E29" s="54"/>
+      <c r="F29" s="54"/>
+      <c r="G29" s="76"/>
+    </row>
+    <row r="30" spans="1:7" ht="56.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="48"/>
+      <c r="B30" s="49"/>
+      <c r="C30" s="58"/>
+      <c r="D30" s="58"/>
+      <c r="E30" s="59"/>
+      <c r="F30" s="60"/>
+      <c r="G30" s="78"/>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A31" s="53"/>
+      <c r="B31" s="54"/>
+      <c r="C31" s="54"/>
+      <c r="D31" s="54"/>
+      <c r="E31" s="54"/>
+      <c r="F31" s="54"/>
+      <c r="G31" s="76"/>
+    </row>
+    <row r="32" spans="1:7" ht="69" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="48"/>
+      <c r="B32" s="49"/>
+      <c r="C32" s="49"/>
+      <c r="D32" s="58"/>
+      <c r="E32" s="50"/>
+      <c r="F32" s="51"/>
+      <c r="G32" s="78"/>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A33" s="53"/>
+      <c r="B33" s="54"/>
+      <c r="C33" s="54"/>
+      <c r="D33" s="54"/>
+      <c r="E33" s="54"/>
+      <c r="F33" s="54"/>
+      <c r="G33" s="76"/>
+    </row>
+    <row r="34" spans="1:7" ht="58.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="48"/>
+      <c r="B34" s="49"/>
+      <c r="C34" s="49"/>
+      <c r="D34" s="58"/>
+      <c r="E34" s="50"/>
+      <c r="F34" s="51"/>
+      <c r="G34" s="78"/>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A35" s="53"/>
+      <c r="B35" s="54"/>
+      <c r="C35" s="54"/>
+      <c r="D35" s="54"/>
+      <c r="E35" s="54"/>
+      <c r="F35" s="54"/>
+      <c r="G35" s="76"/>
+    </row>
+    <row r="36" spans="1:7" ht="54" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A36" s="48"/>
+      <c r="B36" s="49"/>
+      <c r="C36" s="49"/>
+      <c r="D36" s="58"/>
+      <c r="E36" s="50"/>
+      <c r="F36" s="51"/>
+      <c r="G36" s="78"/>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A37" s="53"/>
+      <c r="B37" s="54"/>
+      <c r="C37" s="54"/>
+      <c r="D37" s="54"/>
+      <c r="E37" s="54"/>
+      <c r="F37" s="54"/>
+      <c r="G37" s="76"/>
+    </row>
+    <row r="38" spans="1:7" ht="63.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A38" s="48"/>
+      <c r="B38" s="49"/>
+      <c r="C38" s="49"/>
+      <c r="D38" s="58"/>
+      <c r="E38" s="50"/>
+      <c r="F38" s="51"/>
+      <c r="G38" s="78"/>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A39" s="53"/>
+      <c r="B39" s="54"/>
+      <c r="C39" s="54"/>
+      <c r="D39" s="54"/>
+      <c r="E39" s="54"/>
+      <c r="F39" s="54"/>
+      <c r="G39" s="76"/>
+    </row>
+    <row r="40" spans="1:7" ht="61.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A40" s="48"/>
+      <c r="B40" s="49"/>
+      <c r="C40" s="49"/>
+      <c r="D40" s="58"/>
+      <c r="E40" s="50"/>
+      <c r="F40" s="51"/>
+      <c r="G40" s="78"/>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A41" s="65"/>
+      <c r="B41" s="66"/>
+      <c r="C41" s="66"/>
+      <c r="D41" s="66"/>
+      <c r="E41" s="66"/>
+      <c r="F41" s="66"/>
+      <c r="G41" s="79"/>
+    </row>
+    <row r="42" spans="1:7" ht="64.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A42" s="48"/>
+      <c r="B42" s="49"/>
+      <c r="C42" s="49"/>
+      <c r="D42" s="58"/>
+      <c r="E42" s="50"/>
+      <c r="F42" s="51"/>
+      <c r="G42" s="78"/>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A43" s="65"/>
+      <c r="B43" s="66"/>
+      <c r="C43" s="66"/>
+      <c r="D43" s="66"/>
+      <c r="E43" s="66"/>
+      <c r="F43" s="66"/>
+      <c r="G43" s="79"/>
+    </row>
+    <row r="44" spans="1:7" ht="57.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A44" s="48"/>
+      <c r="B44" s="58"/>
+      <c r="C44" s="58"/>
+      <c r="D44" s="58"/>
+      <c r="E44" s="59"/>
+      <c r="F44" s="60"/>
+      <c r="G44" s="78"/>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A45" s="65"/>
+    </row>
+    <row r="46" spans="1:7" ht="60" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A46" s="48"/>
+      <c r="B46" s="58"/>
+      <c r="C46" s="58"/>
+      <c r="D46" s="58"/>
+      <c r="E46" s="59"/>
+      <c r="F46" s="60"/>
+      <c r="G46" s="78"/>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A47" s="65"/>
+    </row>
+    <row r="48" spans="1:7" ht="58.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A48" s="48"/>
+      <c r="B48" s="58"/>
+      <c r="C48" s="58"/>
+      <c r="D48" s="58"/>
+      <c r="E48" s="59"/>
+      <c r="F48" s="60"/>
+      <c r="G48" s="78"/>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A49" s="65"/>
+    </row>
+    <row r="50" spans="1:7" ht="55.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A50" s="48"/>
+      <c r="B50" s="58"/>
+      <c r="C50" s="58"/>
+      <c r="D50" s="58"/>
+      <c r="E50" s="59"/>
+      <c r="F50" s="60"/>
+      <c r="G50" s="78"/>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A51" s="65"/>
+    </row>
+    <row r="52" spans="1:7" ht="55.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A52" s="48"/>
+      <c r="B52" s="49"/>
+      <c r="C52" s="49"/>
+      <c r="D52" s="49"/>
+      <c r="E52" s="50"/>
+      <c r="F52" s="51"/>
+      <c r="G52" s="78"/>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A53" s="65"/>
+    </row>
+    <row r="54" spans="1:7" ht="51.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A54" s="48"/>
+      <c r="B54" s="49"/>
+      <c r="C54" s="49"/>
+      <c r="D54" s="49"/>
+      <c r="E54" s="50"/>
+      <c r="F54" s="51"/>
+      <c r="G54" s="78"/>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A55" s="65"/>
+    </row>
+    <row r="56" spans="1:7" ht="52.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A56" s="48"/>
+      <c r="B56" s="49"/>
+      <c r="C56" s="49"/>
+      <c r="D56" s="49"/>
+      <c r="E56" s="50"/>
+      <c r="F56" s="51"/>
+      <c r="G56" s="78"/>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A57" s="65"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B3:D3"/>
+  </mergeCells>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G57"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="17" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="28.42578125" customWidth="1"/>
+    <col min="5" max="5" width="33.42578125" customWidth="1"/>
+    <col min="6" max="6" width="25.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="26.7109375" style="80" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="25" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="26" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="27"/>
+      <c r="D1" s="28" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" s="29" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="30" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" s="31" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="32" t="s">
+        <v>163</v>
+      </c>
+      <c r="C2" s="33"/>
+      <c r="D2" s="34"/>
+      <c r="E2" s="35" t="s">
+        <v>59</v>
+      </c>
+      <c r="F2" s="36"/>
+      <c r="G2" s="73"/>
+    </row>
+    <row r="3" spans="1:7" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="25" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="81" t="s">
+        <v>129</v>
+      </c>
+      <c r="C3" s="81"/>
+      <c r="D3" s="81"/>
+      <c r="E3" s="38"/>
+      <c r="F3" s="39"/>
+      <c r="G3" s="73"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E4" s="40"/>
+      <c r="F4" s="41"/>
+      <c r="G4" s="74"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" s="43" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="44" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="43" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" s="43" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5" s="45" t="s">
+        <v>17</v>
+      </c>
+      <c r="F5" s="46" t="s">
+        <v>18</v>
+      </c>
+      <c r="G5" s="47" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="97.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="48" t="s">
+        <v>123</v>
+      </c>
+      <c r="B6" s="49" t="s">
+        <v>124</v>
+      </c>
+      <c r="C6" s="49" t="s">
+        <v>125</v>
+      </c>
+      <c r="D6" s="49" t="s">
+        <v>126</v>
+      </c>
+      <c r="E6" s="50" t="s">
+        <v>127</v>
+      </c>
+      <c r="F6" s="51" t="s">
+        <v>128</v>
+      </c>
+      <c r="G6" s="75" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7" s="53"/>
+      <c r="B7" s="54"/>
+      <c r="C7" s="54"/>
+      <c r="D7" s="54"/>
+      <c r="E7" s="54"/>
+      <c r="F7" s="54"/>
+      <c r="G7" s="76"/>
+    </row>
+    <row r="8" spans="1:7" ht="97.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="48" t="s">
+        <v>159</v>
+      </c>
+      <c r="B8" s="49" t="s">
+        <v>160</v>
+      </c>
+      <c r="C8" s="49" t="s">
+        <v>125</v>
+      </c>
+      <c r="D8" s="49" t="s">
+        <v>126</v>
+      </c>
+      <c r="E8" s="50" t="s">
+        <v>161</v>
+      </c>
+      <c r="F8" s="51" t="s">
+        <v>128</v>
+      </c>
+      <c r="G8" s="77" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9" s="53"/>
+      <c r="B9" s="54"/>
+      <c r="C9" s="54"/>
+      <c r="D9" s="54"/>
+      <c r="E9" s="54"/>
+      <c r="F9" s="54"/>
+      <c r="G9" s="76"/>
+    </row>
+    <row r="10" spans="1:7" ht="72.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="48"/>
       <c r="B10" s="49"/>
       <c r="C10" s="49"/>

</xml_diff>

<commit_message>
Adicionado novos casos de testes para Cdastro de visitante
</commit_message>
<xml_diff>
--- a/testes/cmproject_test_case.xlsx
+++ b/testes/cmproject_test_case.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="990" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="990" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Capa" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="169">
   <si>
     <t>Projeto de Teste</t>
   </si>
@@ -463,6 +463,81 @@
   </si>
   <si>
     <t>CT-b003</t>
+  </si>
+  <si>
+    <t>Fazer cadastro com campo "E-mail" vazios</t>
+  </si>
+  <si>
+    <t>Clicar na opção "Acessos" em seguida clicar em "Cadastre-se" e tentar cadastrar sem preencher o campo "E-mail"</t>
+  </si>
+  <si>
+    <t>Mensagem de "Insira um e-mail válido"</t>
+  </si>
+  <si>
+    <t>Fazer cadastro com campo "Senha" vazios</t>
+  </si>
+  <si>
+    <t>Clicar na opção "Acessos" em seguida clicar em "Cadastre-se" e tentar cadastrar sem preencher o campo "Senha"</t>
+  </si>
+  <si>
+    <t>Mensagem de "Senha Obrigatória"</t>
+  </si>
+  <si>
+    <t>Fazer cadastro com campo "Cpf" vazios</t>
+  </si>
+  <si>
+    <t>Clicar na opção "Acessos" em seguida clicar em "Cadastre-se" e tentar cadastrar sem preencher o campo "Cpf"</t>
+  </si>
+  <si>
+    <t>Mensagem de "Insira seu CPF"</t>
+  </si>
+  <si>
+    <t>Fazer cadastro com campo "Telefone" vazios</t>
+  </si>
+  <si>
+    <t>Clicar na opção "Acessos" em seguida clicar em "Cadastre-se" e tentar cadastrar sem preencher o campo "Telefone"</t>
+  </si>
+  <si>
+    <t>Mensagem de "Insira um telefone"</t>
+  </si>
+  <si>
+    <t>Fazer cadastro com campo "Endereço" vazios</t>
+  </si>
+  <si>
+    <t>Clicar na opção "Acessos" em seguida clicar em "Cadastre-se" e tentar cadastrar sem preencher o campo "Endereço"</t>
+  </si>
+  <si>
+    <t>Mensagem de "Insira um endereço"</t>
+  </si>
+  <si>
+    <t>Fazer cadastro com todos campos preenchidos corretamente</t>
+  </si>
+  <si>
+    <t>Clicar na opção "Acessos" em seguida clicar em "Cadastre-se"  preencher todos os campos corretamente e clicar no botão "Cadastre-se"</t>
+  </si>
+  <si>
+    <t>Mensagem de "Cadastrado com sucesso!"</t>
+  </si>
+  <si>
+    <t>preencher os inputs de acordo com os lables</t>
+  </si>
+  <si>
+    <t>CT-c005</t>
+  </si>
+  <si>
+    <t>CT-c006</t>
+  </si>
+  <si>
+    <t>CT-c007</t>
+  </si>
+  <si>
+    <t>CT-c008</t>
+  </si>
+  <si>
+    <t>CT-c009</t>
+  </si>
+  <si>
+    <t>CT-c010</t>
   </si>
 </sst>
 </file>
@@ -838,7 +913,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="83">
+  <cellXfs count="84">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1006,6 +1081,21 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="13" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1029,18 +1119,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="13" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1545,11 +1623,11 @@
       <c r="B13" s="4"/>
       <c r="C13" s="5"/>
       <c r="D13" s="10"/>
-      <c r="E13" s="71" t="s">
+      <c r="E13" s="76" t="s">
         <v>0</v>
       </c>
-      <c r="F13" s="71"/>
-      <c r="G13" s="71"/>
+      <c r="F13" s="76"/>
+      <c r="G13" s="76"/>
       <c r="H13" s="11"/>
       <c r="I13" s="5"/>
       <c r="J13" s="6"/>
@@ -1558,9 +1636,9 @@
       <c r="B14" s="4"/>
       <c r="C14" s="5"/>
       <c r="D14" s="10"/>
-      <c r="E14" s="71"/>
-      <c r="F14" s="71"/>
-      <c r="G14" s="71"/>
+      <c r="E14" s="76"/>
+      <c r="F14" s="76"/>
+      <c r="G14" s="76"/>
       <c r="H14" s="11"/>
       <c r="I14" s="5"/>
       <c r="J14" s="6"/>
@@ -1580,11 +1658,11 @@
       <c r="B16" s="4"/>
       <c r="C16" s="5"/>
       <c r="D16" s="10"/>
-      <c r="E16" s="72" t="s">
+      <c r="E16" s="77" t="s">
         <v>1</v>
       </c>
-      <c r="F16" s="72"/>
-      <c r="G16" s="72"/>
+      <c r="F16" s="77"/>
+      <c r="G16" s="77"/>
       <c r="H16" s="11"/>
       <c r="I16" s="5"/>
       <c r="J16" s="6"/>
@@ -1593,9 +1671,9 @@
       <c r="B17" s="4"/>
       <c r="C17" s="5"/>
       <c r="D17" s="10"/>
-      <c r="E17" s="72"/>
-      <c r="F17" s="72"/>
-      <c r="G17" s="72"/>
+      <c r="E17" s="77"/>
+      <c r="F17" s="77"/>
+      <c r="G17" s="77"/>
       <c r="H17" s="11"/>
       <c r="I17" s="5"/>
       <c r="J17" s="6"/>
@@ -1641,11 +1719,11 @@
       <c r="B21" s="4"/>
       <c r="C21" s="5"/>
       <c r="D21" s="10"/>
-      <c r="E21" s="73" t="s">
+      <c r="E21" s="78" t="s">
         <v>4</v>
       </c>
-      <c r="F21" s="73"/>
-      <c r="G21" s="73"/>
+      <c r="F21" s="78"/>
+      <c r="G21" s="78"/>
       <c r="H21" s="11"/>
       <c r="I21" s="5"/>
       <c r="J21" s="6"/>
@@ -1654,11 +1732,11 @@
       <c r="B22" s="4"/>
       <c r="C22" s="5"/>
       <c r="D22" s="10"/>
-      <c r="E22" s="73" t="s">
+      <c r="E22" s="78" t="s">
         <v>5</v>
       </c>
-      <c r="F22" s="73"/>
-      <c r="G22" s="73"/>
+      <c r="F22" s="78"/>
+      <c r="G22" s="78"/>
       <c r="H22" s="11"/>
       <c r="I22" s="5"/>
       <c r="J22" s="6"/>
@@ -1667,9 +1745,9 @@
       <c r="B23" s="4"/>
       <c r="C23" s="5"/>
       <c r="D23" s="10"/>
-      <c r="E23" s="74"/>
-      <c r="F23" s="74"/>
-      <c r="G23" s="74"/>
+      <c r="E23" s="79"/>
+      <c r="F23" s="79"/>
+      <c r="G23" s="79"/>
       <c r="H23" s="11"/>
       <c r="I23" s="5"/>
       <c r="J23" s="6"/>
@@ -1897,11 +1975,11 @@
       <c r="A3" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="75" t="s">
+      <c r="B3" s="80" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="75"/>
-      <c r="D3" s="75"/>
+      <c r="C3" s="80"/>
+      <c r="D3" s="80"/>
       <c r="E3" s="34"/>
       <c r="F3" s="35"/>
       <c r="G3" s="33"/>
@@ -2608,7 +2686,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
@@ -2664,11 +2742,11 @@
       <c r="A3" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="75" t="s">
+      <c r="B3" s="80" t="s">
         <v>65</v>
       </c>
-      <c r="C3" s="75"/>
-      <c r="D3" s="75"/>
+      <c r="C3" s="80"/>
+      <c r="D3" s="80"/>
       <c r="E3" s="34"/>
       <c r="F3" s="35"/>
       <c r="G3" s="33"/>
@@ -2720,7 +2798,7 @@
       <c r="F6" s="47" t="s">
         <v>71</v>
       </c>
-      <c r="G6" s="82" t="s">
+      <c r="G6" s="75" t="s">
         <v>72</v>
       </c>
     </row>
@@ -2752,7 +2830,7 @@
       <c r="F8" s="47" t="s">
         <v>77</v>
       </c>
-      <c r="G8" s="82" t="s">
+      <c r="G8" s="75" t="s">
         <v>78</v>
       </c>
     </row>
@@ -2778,13 +2856,13 @@
       <c r="D10" s="44" t="s">
         <v>141</v>
       </c>
-      <c r="E10" s="79" t="s">
+      <c r="E10" s="72" t="s">
         <v>142</v>
       </c>
-      <c r="F10" s="80" t="s">
+      <c r="F10" s="73" t="s">
         <v>140</v>
       </c>
-      <c r="G10" s="81" t="s">
+      <c r="G10" s="74" t="s">
         <v>142</v>
       </c>
     </row>
@@ -3031,10 +3109,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G20"/>
+  <dimension ref="A1:G24"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B6" sqref="A6:XFD6"/>
+    <sheetView tabSelected="1" topLeftCell="A15" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3089,11 +3167,11 @@
       <c r="A3" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="76" t="s">
+      <c r="B3" s="81" t="s">
         <v>80</v>
       </c>
-      <c r="C3" s="76"/>
-      <c r="D3" s="76"/>
+      <c r="C3" s="81"/>
+      <c r="D3" s="81"/>
       <c r="E3" s="34"/>
       <c r="F3" s="35"/>
       <c r="G3" s="66"/>
@@ -3133,8 +3211,8 @@
       <c r="B6" s="45" t="s">
         <v>82</v>
       </c>
-      <c r="C6" s="45" t="s">
-        <v>83</v>
+      <c r="C6" s="71" t="s">
+        <v>140</v>
       </c>
       <c r="D6" s="45" t="s">
         <v>84</v>
@@ -3254,14 +3332,28 @@
       <c r="F13" s="50"/>
       <c r="G13" s="68"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A14" s="44"/>
-      <c r="B14" s="45"/>
-      <c r="C14" s="45"/>
-      <c r="D14" s="45"/>
-      <c r="E14" s="46"/>
-      <c r="F14" s="47"/>
-      <c r="G14" s="69"/>
+    <row r="14" spans="1:7" ht="51" x14ac:dyDescent="0.2">
+      <c r="A14" s="71" t="s">
+        <v>163</v>
+      </c>
+      <c r="B14" s="71" t="s">
+        <v>144</v>
+      </c>
+      <c r="C14" s="71" t="s">
+        <v>140</v>
+      </c>
+      <c r="D14" s="71" t="s">
+        <v>145</v>
+      </c>
+      <c r="E14" s="72" t="s">
+        <v>146</v>
+      </c>
+      <c r="F14" s="73" t="s">
+        <v>140</v>
+      </c>
+      <c r="G14" s="74" t="s">
+        <v>146</v>
+      </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" s="49"/>
@@ -3272,17 +3364,31 @@
       <c r="F15" s="50"/>
       <c r="G15" s="68"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A16" s="44"/>
-      <c r="B16" s="45"/>
-      <c r="C16" s="45"/>
-      <c r="D16" s="45"/>
-      <c r="E16" s="46"/>
-      <c r="F16" s="52"/>
-      <c r="G16" s="69"/>
+    <row r="16" spans="1:7" ht="51" x14ac:dyDescent="0.2">
+      <c r="A16" s="71" t="s">
+        <v>164</v>
+      </c>
+      <c r="B16" s="71" t="s">
+        <v>147</v>
+      </c>
+      <c r="C16" s="71" t="s">
+        <v>140</v>
+      </c>
+      <c r="D16" s="71" t="s">
+        <v>148</v>
+      </c>
+      <c r="E16" s="72" t="s">
+        <v>149</v>
+      </c>
+      <c r="F16" s="73" t="s">
+        <v>140</v>
+      </c>
+      <c r="G16" s="74" t="s">
+        <v>149</v>
+      </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A17" s="49"/>
+      <c r="A17" s="54"/>
       <c r="B17" s="50"/>
       <c r="C17" s="50"/>
       <c r="D17" s="50"/>
@@ -3290,32 +3396,124 @@
       <c r="F17" s="50"/>
       <c r="G17" s="68"/>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A18" s="44"/>
-      <c r="B18" s="45"/>
-      <c r="C18" s="45"/>
-      <c r="D18" s="45"/>
-      <c r="E18" s="46"/>
-      <c r="F18" s="52"/>
-      <c r="G18" s="69"/>
+    <row r="18" spans="1:7" ht="51" x14ac:dyDescent="0.2">
+      <c r="A18" s="71" t="s">
+        <v>165</v>
+      </c>
+      <c r="B18" s="71" t="s">
+        <v>150</v>
+      </c>
+      <c r="C18" s="71" t="s">
+        <v>140</v>
+      </c>
+      <c r="D18" s="71" t="s">
+        <v>151</v>
+      </c>
+      <c r="E18" s="72" t="s">
+        <v>152</v>
+      </c>
+      <c r="F18" s="73" t="s">
+        <v>140</v>
+      </c>
+      <c r="G18" s="74" t="s">
+        <v>152</v>
+      </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A19" s="54"/>
-      <c r="B19" s="50"/>
+      <c r="A19" s="59"/>
+      <c r="B19" s="60"/>
       <c r="C19" s="50"/>
       <c r="D19" s="50"/>
       <c r="E19" s="50"/>
       <c r="F19" s="50"/>
       <c r="G19" s="68"/>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A20" s="44"/>
-      <c r="B20" s="55"/>
-      <c r="C20" s="55"/>
-      <c r="D20" s="55"/>
-      <c r="E20" s="56"/>
-      <c r="F20" s="57"/>
-      <c r="G20" s="69"/>
+    <row r="20" spans="1:7" ht="51" x14ac:dyDescent="0.2">
+      <c r="A20" s="71" t="s">
+        <v>166</v>
+      </c>
+      <c r="B20" s="71" t="s">
+        <v>153</v>
+      </c>
+      <c r="C20" s="71" t="s">
+        <v>140</v>
+      </c>
+      <c r="D20" s="71" t="s">
+        <v>154</v>
+      </c>
+      <c r="E20" s="72" t="s">
+        <v>155</v>
+      </c>
+      <c r="F20" s="73" t="s">
+        <v>140</v>
+      </c>
+      <c r="G20" s="74" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A21" s="61"/>
+      <c r="B21" s="60"/>
+      <c r="C21" s="50"/>
+      <c r="D21" s="50"/>
+      <c r="E21" s="50"/>
+      <c r="F21" s="50"/>
+      <c r="G21" s="68"/>
+    </row>
+    <row r="22" spans="1:7" ht="51" x14ac:dyDescent="0.2">
+      <c r="A22" s="71" t="s">
+        <v>167</v>
+      </c>
+      <c r="B22" s="71" t="s">
+        <v>156</v>
+      </c>
+      <c r="C22" s="71" t="s">
+        <v>140</v>
+      </c>
+      <c r="D22" s="71" t="s">
+        <v>157</v>
+      </c>
+      <c r="E22" s="72" t="s">
+        <v>158</v>
+      </c>
+      <c r="F22" s="73" t="s">
+        <v>140</v>
+      </c>
+      <c r="G22" s="74" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A23" s="61"/>
+      <c r="B23" s="60"/>
+      <c r="C23" s="50"/>
+      <c r="D23" s="50"/>
+      <c r="E23" s="50"/>
+      <c r="F23" s="50"/>
+      <c r="G23" s="68"/>
+    </row>
+    <row r="24" spans="1:7" ht="63.75" x14ac:dyDescent="0.2">
+      <c r="A24" s="71" t="s">
+        <v>168</v>
+      </c>
+      <c r="B24" s="71" t="s">
+        <v>159</v>
+      </c>
+      <c r="C24" s="71" t="s">
+        <v>140</v>
+      </c>
+      <c r="D24" s="71" t="s">
+        <v>160</v>
+      </c>
+      <c r="E24" s="72" t="s">
+        <v>161</v>
+      </c>
+      <c r="F24" s="73" t="s">
+        <v>162</v>
+      </c>
+      <c r="G24" s="74" t="s">
+        <v>161</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -3386,11 +3584,11 @@
       <c r="A3" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="77" t="s">
+      <c r="B3" s="82" t="s">
         <v>104</v>
       </c>
-      <c r="C3" s="77"/>
-      <c r="D3" s="77"/>
+      <c r="C3" s="82"/>
+      <c r="D3" s="82"/>
       <c r="E3" s="34"/>
       <c r="F3" s="35"/>
       <c r="G3" s="66"/>
@@ -3665,11 +3863,11 @@
       <c r="A3" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="78" t="s">
+      <c r="B3" s="83" t="s">
         <v>104</v>
       </c>
-      <c r="C3" s="78"/>
-      <c r="D3" s="78"/>
+      <c r="C3" s="83"/>
+      <c r="D3" s="83"/>
       <c r="E3" s="34"/>
       <c r="F3" s="35"/>
       <c r="G3" s="66"/>

</xml_diff>

<commit_message>
Adicionado novos casos de testes para cadastro de colaborador
</commit_message>
<xml_diff>
--- a/testes/cmproject_test_case.xlsx
+++ b/testes/cmproject_test_case.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="990" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="990" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Capa" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="354" uniqueCount="184">
   <si>
     <t>Projeto de Teste</t>
   </si>
@@ -538,6 +538,51 @@
   </si>
   <si>
     <t>CT-c010</t>
+  </si>
+  <si>
+    <t>Fazer cadastro de administrador com campo "Nome" vazios</t>
+  </si>
+  <si>
+    <t>Clicar na opção "Acessos" em seguida clicar em "Ações Administrativas" e em seguida clicar em "Cadastrar colaborador" e tentar cadastrar sem preencher o campo "Nome"</t>
+  </si>
+  <si>
+    <t>Mensagem de "Campo Nome Obrigatório"</t>
+  </si>
+  <si>
+    <t>Fazer cadastro de administrador com campo "E-mail" vazios</t>
+  </si>
+  <si>
+    <t>Clicar na opção "Acessos" em seguida clicar em  "Ações Administrativas" e em seguida clicar em "Cadastrar colaborador" e tentar cadastrar sem preencher o campo "E-mail"</t>
+  </si>
+  <si>
+    <t>Fazer cadastro de administrador com campo "Senha" vazios</t>
+  </si>
+  <si>
+    <t>Clicar na opção "Acessos" em seguida clicar em  "Ações Administrativas" e em seguida clicar em "Cadastrar colaborador" e tentar cadastrar sem preencher o campo "Senha"</t>
+  </si>
+  <si>
+    <t>Fazer cadastro de administrador com campo "Cpf" vazios</t>
+  </si>
+  <si>
+    <t>Fazer cadastro de administrador com campo "Telefone" vazios</t>
+  </si>
+  <si>
+    <t>Clicar na opção "Acessos" em seguida clicar em  "Ações Administrativas" e em seguida clicar em "Cadastrar colaborador" e tentar cadastrar sem preencher o campo "Telefone"</t>
+  </si>
+  <si>
+    <t>Fazer cadastro de administrador com campo "Endereço" vazios</t>
+  </si>
+  <si>
+    <t>Clicar na opção "Acessos" em seguida clicar em  "Ações Administrativas" e em seguida clicar em "Cadastrar colaborador" e tentar cadastrar sem preencher o campo "Endereço"</t>
+  </si>
+  <si>
+    <t>Fazer cadastro de administrador com todos campos preenchidos corretamente</t>
+  </si>
+  <si>
+    <t>Clicar na opção "Acessos" em seguida clicar em  "Ações Administrativas" e em seguida clicar em "Cadastro colaborador"  preencher todos os campos corretamente e clicar no botão "Cadastrar"</t>
+  </si>
+  <si>
+    <t>CT-c011</t>
   </si>
 </sst>
 </file>
@@ -913,7 +958,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="84">
+  <cellXfs count="86">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1096,6 +1141,9 @@
     <xf numFmtId="0" fontId="10" fillId="13" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1119,6 +1167,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1623,11 +1674,11 @@
       <c r="B13" s="4"/>
       <c r="C13" s="5"/>
       <c r="D13" s="10"/>
-      <c r="E13" s="76" t="s">
+      <c r="E13" s="77" t="s">
         <v>0</v>
       </c>
-      <c r="F13" s="76"/>
-      <c r="G13" s="76"/>
+      <c r="F13" s="77"/>
+      <c r="G13" s="77"/>
       <c r="H13" s="11"/>
       <c r="I13" s="5"/>
       <c r="J13" s="6"/>
@@ -1636,9 +1687,9 @@
       <c r="B14" s="4"/>
       <c r="C14" s="5"/>
       <c r="D14" s="10"/>
-      <c r="E14" s="76"/>
-      <c r="F14" s="76"/>
-      <c r="G14" s="76"/>
+      <c r="E14" s="77"/>
+      <c r="F14" s="77"/>
+      <c r="G14" s="77"/>
       <c r="H14" s="11"/>
       <c r="I14" s="5"/>
       <c r="J14" s="6"/>
@@ -1658,11 +1709,11 @@
       <c r="B16" s="4"/>
       <c r="C16" s="5"/>
       <c r="D16" s="10"/>
-      <c r="E16" s="77" t="s">
+      <c r="E16" s="78" t="s">
         <v>1</v>
       </c>
-      <c r="F16" s="77"/>
-      <c r="G16" s="77"/>
+      <c r="F16" s="78"/>
+      <c r="G16" s="78"/>
       <c r="H16" s="11"/>
       <c r="I16" s="5"/>
       <c r="J16" s="6"/>
@@ -1671,9 +1722,9 @@
       <c r="B17" s="4"/>
       <c r="C17" s="5"/>
       <c r="D17" s="10"/>
-      <c r="E17" s="77"/>
-      <c r="F17" s="77"/>
-      <c r="G17" s="77"/>
+      <c r="E17" s="78"/>
+      <c r="F17" s="78"/>
+      <c r="G17" s="78"/>
       <c r="H17" s="11"/>
       <c r="I17" s="5"/>
       <c r="J17" s="6"/>
@@ -1719,11 +1770,11 @@
       <c r="B21" s="4"/>
       <c r="C21" s="5"/>
       <c r="D21" s="10"/>
-      <c r="E21" s="78" t="s">
+      <c r="E21" s="79" t="s">
         <v>4</v>
       </c>
-      <c r="F21" s="78"/>
-      <c r="G21" s="78"/>
+      <c r="F21" s="79"/>
+      <c r="G21" s="79"/>
       <c r="H21" s="11"/>
       <c r="I21" s="5"/>
       <c r="J21" s="6"/>
@@ -1732,11 +1783,11 @@
       <c r="B22" s="4"/>
       <c r="C22" s="5"/>
       <c r="D22" s="10"/>
-      <c r="E22" s="78" t="s">
+      <c r="E22" s="79" t="s">
         <v>5</v>
       </c>
-      <c r="F22" s="78"/>
-      <c r="G22" s="78"/>
+      <c r="F22" s="79"/>
+      <c r="G22" s="79"/>
       <c r="H22" s="11"/>
       <c r="I22" s="5"/>
       <c r="J22" s="6"/>
@@ -1745,9 +1796,9 @@
       <c r="B23" s="4"/>
       <c r="C23" s="5"/>
       <c r="D23" s="10"/>
-      <c r="E23" s="79"/>
-      <c r="F23" s="79"/>
-      <c r="G23" s="79"/>
+      <c r="E23" s="80"/>
+      <c r="F23" s="80"/>
+      <c r="G23" s="80"/>
       <c r="H23" s="11"/>
       <c r="I23" s="5"/>
       <c r="J23" s="6"/>
@@ -1975,11 +2026,11 @@
       <c r="A3" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="80" t="s">
+      <c r="B3" s="81" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="80"/>
-      <c r="D3" s="80"/>
+      <c r="C3" s="81"/>
+      <c r="D3" s="81"/>
       <c r="E3" s="34"/>
       <c r="F3" s="35"/>
       <c r="G3" s="33"/>
@@ -2742,11 +2793,11 @@
       <c r="A3" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="80" t="s">
+      <c r="B3" s="81" t="s">
         <v>65</v>
       </c>
-      <c r="C3" s="80"/>
-      <c r="D3" s="80"/>
+      <c r="C3" s="81"/>
+      <c r="D3" s="81"/>
       <c r="E3" s="34"/>
       <c r="F3" s="35"/>
       <c r="G3" s="33"/>
@@ -3111,7 +3162,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A15" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
@@ -3167,11 +3218,11 @@
       <c r="A3" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="81" t="s">
+      <c r="B3" s="82" t="s">
         <v>80</v>
       </c>
-      <c r="C3" s="81"/>
-      <c r="D3" s="81"/>
+      <c r="C3" s="82"/>
+      <c r="D3" s="82"/>
       <c r="E3" s="34"/>
       <c r="F3" s="35"/>
       <c r="G3" s="66"/>
@@ -3526,10 +3577,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G18"/>
+  <dimension ref="A1:G26"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D1" activeCellId="1" sqref="A6:XFD6 D1"/>
+    <sheetView topLeftCell="A21" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3584,11 +3635,11 @@
       <c r="A3" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="82" t="s">
+      <c r="B3" s="83" t="s">
         <v>104</v>
       </c>
-      <c r="C3" s="82"/>
-      <c r="D3" s="82"/>
+      <c r="C3" s="83"/>
+      <c r="D3" s="83"/>
       <c r="E3" s="34"/>
       <c r="F3" s="35"/>
       <c r="G3" s="66"/>
@@ -3749,32 +3800,60 @@
       <c r="F13" s="50"/>
       <c r="G13" s="68"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A14" s="44"/>
-      <c r="B14" s="45"/>
-      <c r="C14" s="45"/>
-      <c r="D14" s="45"/>
-      <c r="E14" s="46"/>
-      <c r="F14" s="47"/>
-      <c r="G14" s="69"/>
+    <row r="14" spans="1:7" ht="76.5" x14ac:dyDescent="0.2">
+      <c r="A14" s="76" t="s">
+        <v>163</v>
+      </c>
+      <c r="B14" s="76" t="s">
+        <v>169</v>
+      </c>
+      <c r="C14" s="76" t="s">
+        <v>140</v>
+      </c>
+      <c r="D14" s="76" t="s">
+        <v>170</v>
+      </c>
+      <c r="E14" s="72" t="s">
+        <v>171</v>
+      </c>
+      <c r="F14" s="73" t="s">
+        <v>140</v>
+      </c>
+      <c r="G14" s="74" t="s">
+        <v>171</v>
+      </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" s="49"/>
-      <c r="B15" s="50"/>
-      <c r="C15" s="50"/>
-      <c r="D15" s="50"/>
-      <c r="E15" s="50"/>
-      <c r="F15" s="50"/>
-      <c r="G15" s="68"/>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A16" s="44"/>
-      <c r="B16" s="45"/>
-      <c r="C16" s="45"/>
-      <c r="D16" s="45"/>
-      <c r="E16" s="46"/>
-      <c r="F16" s="52"/>
-      <c r="G16" s="69"/>
+      <c r="B15" s="49"/>
+      <c r="C15" s="49"/>
+      <c r="D15" s="49"/>
+      <c r="E15" s="49"/>
+      <c r="F15" s="49"/>
+      <c r="G15" s="85"/>
+    </row>
+    <row r="16" spans="1:7" ht="89.25" x14ac:dyDescent="0.2">
+      <c r="A16" s="76" t="s">
+        <v>164</v>
+      </c>
+      <c r="B16" s="76" t="s">
+        <v>172</v>
+      </c>
+      <c r="C16" s="76" t="s">
+        <v>140</v>
+      </c>
+      <c r="D16" s="76" t="s">
+        <v>173</v>
+      </c>
+      <c r="E16" s="72" t="s">
+        <v>146</v>
+      </c>
+      <c r="F16" s="73" t="s">
+        <v>140</v>
+      </c>
+      <c r="G16" s="74" t="s">
+        <v>146</v>
+      </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" s="49"/>
@@ -3785,14 +3864,156 @@
       <c r="F17" s="50"/>
       <c r="G17" s="68"/>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A18" s="44"/>
-      <c r="B18" s="45"/>
-      <c r="C18" s="45"/>
-      <c r="D18" s="45"/>
-      <c r="E18" s="46"/>
-      <c r="F18" s="52"/>
-      <c r="G18" s="69"/>
+    <row r="18" spans="1:7" ht="89.25" x14ac:dyDescent="0.2">
+      <c r="A18" s="76" t="s">
+        <v>165</v>
+      </c>
+      <c r="B18" s="76" t="s">
+        <v>174</v>
+      </c>
+      <c r="C18" s="76" t="s">
+        <v>140</v>
+      </c>
+      <c r="D18" s="76" t="s">
+        <v>175</v>
+      </c>
+      <c r="E18" s="72" t="s">
+        <v>149</v>
+      </c>
+      <c r="F18" s="73" t="s">
+        <v>140</v>
+      </c>
+      <c r="G18" s="74" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A19" s="54"/>
+      <c r="B19" s="50"/>
+      <c r="C19" s="50"/>
+      <c r="D19" s="50"/>
+      <c r="E19" s="50"/>
+      <c r="F19" s="50"/>
+      <c r="G19" s="68"/>
+    </row>
+    <row r="20" spans="1:7" ht="51" x14ac:dyDescent="0.2">
+      <c r="A20" s="76" t="s">
+        <v>166</v>
+      </c>
+      <c r="B20" s="76" t="s">
+        <v>176</v>
+      </c>
+      <c r="C20" s="76" t="s">
+        <v>140</v>
+      </c>
+      <c r="D20" s="76" t="s">
+        <v>151</v>
+      </c>
+      <c r="E20" s="72" t="s">
+        <v>152</v>
+      </c>
+      <c r="F20" s="73" t="s">
+        <v>140</v>
+      </c>
+      <c r="G20" s="74" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A21" s="59"/>
+      <c r="B21" s="60"/>
+      <c r="C21" s="50"/>
+      <c r="D21" s="50"/>
+      <c r="E21" s="50"/>
+      <c r="F21" s="50"/>
+      <c r="G21" s="68"/>
+    </row>
+    <row r="22" spans="1:7" ht="89.25" x14ac:dyDescent="0.2">
+      <c r="A22" s="76" t="s">
+        <v>167</v>
+      </c>
+      <c r="B22" s="76" t="s">
+        <v>177</v>
+      </c>
+      <c r="C22" s="76" t="s">
+        <v>140</v>
+      </c>
+      <c r="D22" s="76" t="s">
+        <v>178</v>
+      </c>
+      <c r="E22" s="72" t="s">
+        <v>155</v>
+      </c>
+      <c r="F22" s="73" t="s">
+        <v>140</v>
+      </c>
+      <c r="G22" s="74" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A23" s="61"/>
+      <c r="B23" s="60"/>
+      <c r="C23" s="50"/>
+      <c r="D23" s="50"/>
+      <c r="E23" s="50"/>
+      <c r="F23" s="50"/>
+      <c r="G23" s="68"/>
+    </row>
+    <row r="24" spans="1:7" ht="89.25" x14ac:dyDescent="0.2">
+      <c r="A24" s="76" t="s">
+        <v>168</v>
+      </c>
+      <c r="B24" s="76" t="s">
+        <v>179</v>
+      </c>
+      <c r="C24" s="76" t="s">
+        <v>140</v>
+      </c>
+      <c r="D24" s="76" t="s">
+        <v>180</v>
+      </c>
+      <c r="E24" s="72" t="s">
+        <v>158</v>
+      </c>
+      <c r="F24" s="73" t="s">
+        <v>140</v>
+      </c>
+      <c r="G24" s="74" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A25" s="61"/>
+      <c r="B25" s="60"/>
+      <c r="C25" s="50"/>
+      <c r="D25" s="50"/>
+      <c r="E25" s="50"/>
+      <c r="F25" s="50"/>
+      <c r="G25" s="68"/>
+    </row>
+    <row r="26" spans="1:7" ht="89.25" x14ac:dyDescent="0.2">
+      <c r="A26" s="76" t="s">
+        <v>183</v>
+      </c>
+      <c r="B26" s="76" t="s">
+        <v>181</v>
+      </c>
+      <c r="C26" s="76" t="s">
+        <v>140</v>
+      </c>
+      <c r="D26" s="76" t="s">
+        <v>182</v>
+      </c>
+      <c r="E26" s="72" t="s">
+        <v>161</v>
+      </c>
+      <c r="F26" s="73" t="s">
+        <v>162</v>
+      </c>
+      <c r="G26" s="74" t="s">
+        <v>161</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -3807,7 +4028,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G56"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
@@ -3863,11 +4084,11 @@
       <c r="A3" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="83" t="s">
+      <c r="B3" s="84" t="s">
         <v>104</v>
       </c>
-      <c r="C3" s="83"/>
-      <c r="D3" s="83"/>
+      <c r="C3" s="84"/>
+      <c r="D3" s="84"/>
       <c r="E3" s="34"/>
       <c r="F3" s="35"/>
       <c r="G3" s="66"/>

</xml_diff>

<commit_message>
Alteração no caso de teste
</commit_message>
<xml_diff>
--- a/testes/cmproject_test_case.xlsx
+++ b/testes/cmproject_test_case.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="990" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="990" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Capa" sheetId="1" r:id="rId1"/>
@@ -1144,6 +1144,9 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1167,9 +1170,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1674,11 +1674,11 @@
       <c r="B13" s="4"/>
       <c r="C13" s="5"/>
       <c r="D13" s="10"/>
-      <c r="E13" s="77" t="s">
+      <c r="E13" s="78" t="s">
         <v>0</v>
       </c>
-      <c r="F13" s="77"/>
-      <c r="G13" s="77"/>
+      <c r="F13" s="78"/>
+      <c r="G13" s="78"/>
       <c r="H13" s="11"/>
       <c r="I13" s="5"/>
       <c r="J13" s="6"/>
@@ -1687,9 +1687,9 @@
       <c r="B14" s="4"/>
       <c r="C14" s="5"/>
       <c r="D14" s="10"/>
-      <c r="E14" s="77"/>
-      <c r="F14" s="77"/>
-      <c r="G14" s="77"/>
+      <c r="E14" s="78"/>
+      <c r="F14" s="78"/>
+      <c r="G14" s="78"/>
       <c r="H14" s="11"/>
       <c r="I14" s="5"/>
       <c r="J14" s="6"/>
@@ -1709,11 +1709,11 @@
       <c r="B16" s="4"/>
       <c r="C16" s="5"/>
       <c r="D16" s="10"/>
-      <c r="E16" s="78" t="s">
+      <c r="E16" s="79" t="s">
         <v>1</v>
       </c>
-      <c r="F16" s="78"/>
-      <c r="G16" s="78"/>
+      <c r="F16" s="79"/>
+      <c r="G16" s="79"/>
       <c r="H16" s="11"/>
       <c r="I16" s="5"/>
       <c r="J16" s="6"/>
@@ -1722,9 +1722,9 @@
       <c r="B17" s="4"/>
       <c r="C17" s="5"/>
       <c r="D17" s="10"/>
-      <c r="E17" s="78"/>
-      <c r="F17" s="78"/>
-      <c r="G17" s="78"/>
+      <c r="E17" s="79"/>
+      <c r="F17" s="79"/>
+      <c r="G17" s="79"/>
       <c r="H17" s="11"/>
       <c r="I17" s="5"/>
       <c r="J17" s="6"/>
@@ -1770,11 +1770,11 @@
       <c r="B21" s="4"/>
       <c r="C21" s="5"/>
       <c r="D21" s="10"/>
-      <c r="E21" s="79" t="s">
+      <c r="E21" s="80" t="s">
         <v>4</v>
       </c>
-      <c r="F21" s="79"/>
-      <c r="G21" s="79"/>
+      <c r="F21" s="80"/>
+      <c r="G21" s="80"/>
       <c r="H21" s="11"/>
       <c r="I21" s="5"/>
       <c r="J21" s="6"/>
@@ -1783,11 +1783,11 @@
       <c r="B22" s="4"/>
       <c r="C22" s="5"/>
       <c r="D22" s="10"/>
-      <c r="E22" s="79" t="s">
+      <c r="E22" s="80" t="s">
         <v>5</v>
       </c>
-      <c r="F22" s="79"/>
-      <c r="G22" s="79"/>
+      <c r="F22" s="80"/>
+      <c r="G22" s="80"/>
       <c r="H22" s="11"/>
       <c r="I22" s="5"/>
       <c r="J22" s="6"/>
@@ -1796,9 +1796,9 @@
       <c r="B23" s="4"/>
       <c r="C23" s="5"/>
       <c r="D23" s="10"/>
-      <c r="E23" s="80"/>
-      <c r="F23" s="80"/>
-      <c r="G23" s="80"/>
+      <c r="E23" s="81"/>
+      <c r="F23" s="81"/>
+      <c r="G23" s="81"/>
       <c r="H23" s="11"/>
       <c r="I23" s="5"/>
       <c r="J23" s="6"/>
@@ -2026,11 +2026,11 @@
       <c r="A3" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="81" t="s">
+      <c r="B3" s="82" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="81"/>
-      <c r="D3" s="81"/>
+      <c r="C3" s="82"/>
+      <c r="D3" s="82"/>
       <c r="E3" s="34"/>
       <c r="F3" s="35"/>
       <c r="G3" s="33"/>
@@ -2793,11 +2793,11 @@
       <c r="A3" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="81" t="s">
+      <c r="B3" s="82" t="s">
         <v>65</v>
       </c>
-      <c r="C3" s="81"/>
-      <c r="D3" s="81"/>
+      <c r="C3" s="82"/>
+      <c r="D3" s="82"/>
       <c r="E3" s="34"/>
       <c r="F3" s="35"/>
       <c r="G3" s="33"/>
@@ -3218,11 +3218,11 @@
       <c r="A3" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="82" t="s">
+      <c r="B3" s="83" t="s">
         <v>80</v>
       </c>
-      <c r="C3" s="82"/>
-      <c r="D3" s="82"/>
+      <c r="C3" s="83"/>
+      <c r="D3" s="83"/>
       <c r="E3" s="34"/>
       <c r="F3" s="35"/>
       <c r="G3" s="66"/>
@@ -3579,8 +3579,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G26"/>
   <sheetViews>
-    <sheetView topLeftCell="A21" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A27" sqref="A27"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3635,11 +3635,11 @@
       <c r="A3" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="83" t="s">
+      <c r="B3" s="84" t="s">
         <v>104</v>
       </c>
-      <c r="C3" s="83"/>
-      <c r="D3" s="83"/>
+      <c r="C3" s="84"/>
+      <c r="D3" s="84"/>
       <c r="E3" s="34"/>
       <c r="F3" s="35"/>
       <c r="G3" s="66"/>
@@ -3830,7 +3830,7 @@
       <c r="D15" s="49"/>
       <c r="E15" s="49"/>
       <c r="F15" s="49"/>
-      <c r="G15" s="85"/>
+      <c r="G15" s="77"/>
     </row>
     <row r="16" spans="1:7" ht="89.25" x14ac:dyDescent="0.2">
       <c r="A16" s="76" t="s">
@@ -4028,8 +4028,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G56"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4084,11 +4084,11 @@
       <c r="A3" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="84" t="s">
+      <c r="B3" s="85" t="s">
         <v>104</v>
       </c>
-      <c r="C3" s="84"/>
-      <c r="D3" s="84"/>
+      <c r="C3" s="85"/>
+      <c r="D3" s="85"/>
       <c r="E3" s="34"/>
       <c r="F3" s="35"/>
       <c r="G3" s="66"/>

</xml_diff>

<commit_message>
update casos de testes - update resultados anteriores - inserção dos testes da localização da locadora
</commit_message>
<xml_diff>
--- a/testes/cmproject_test_case.xlsx
+++ b/testes/cmproject_test_case.xlsx
@@ -5,20 +5,21 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\PROJETOS SMARTGIT\cmproject\testes\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Documentos\Github\cmproject\testes\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="990" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="851" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Capa" sheetId="1" r:id="rId1"/>
-    <sheet name="Revisão" sheetId="2" r:id="rId2"/>
+    <sheet name="Revisão" sheetId="2" state="hidden" r:id="rId2"/>
     <sheet name="UC - Alugar Veículo" sheetId="3" r:id="rId3"/>
     <sheet name="UC - Login" sheetId="4" r:id="rId4"/>
     <sheet name="UC - Cadastro Visitante" sheetId="5" r:id="rId5"/>
     <sheet name="UC - Cadastro Colaborador" sheetId="6" r:id="rId6"/>
     <sheet name="UC - Cadastrar Veículos" sheetId="7" r:id="rId7"/>
+    <sheet name="UC - Localizar" sheetId="8" r:id="rId8"/>
   </sheets>
   <definedNames>
     <definedName name="LOCAL_MYSQL_DATE_FORMAT" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="354" uniqueCount="184">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="386" uniqueCount="203">
   <si>
     <t>Projeto de Teste</t>
   </si>
@@ -108,10 +109,6 @@
     <t>QUE O SISTEMA RETORNE COM A MENSAGEM DE VEÍCULO ALUGADO</t>
   </si>
   <si>
-    <t>LOGIN: cimara@gmail.com
-SENHA: 1234</t>
-  </si>
-  <si>
     <t>N/A</t>
   </si>
   <si>
@@ -128,9 +125,6 @@
   </si>
   <si>
     <t>ALUGAR VEÍCULO INDISPONÍVEL</t>
-  </si>
-  <si>
-    <t>QUE VEÍCULOS INDISÓNÍVEIS NÃO SEJAM VISÍVEIS PARA O USUÁRIO</t>
   </si>
   <si>
     <t>CT-a004</t>
@@ -583,12 +577,77 @@
   </si>
   <si>
     <t>CT-c011</t>
+  </si>
+  <si>
+    <t>Mensagem: Este veículo foi alugado cmo sucesso!!</t>
+  </si>
+  <si>
+    <t>LOGIN: cimara@gmail.com
+SENHA: 1234
+Data: DD/MM/YYYY</t>
+  </si>
+  <si>
+    <t>Não impede que veículo seja alugado estando em prazo de uso já utilizado.</t>
+  </si>
+  <si>
+    <t>O VISITANTE SELECIONA VEICULO, CLICA EM ALUGAR .</t>
+  </si>
+  <si>
+    <t>QUE VEÍCULOS INDISÓNÍVEIS NÃO ESTEJAM COM O BOTÃO DE ALUGAR DISPONÍVEL</t>
+  </si>
+  <si>
+    <t>Função alugar indisponível para o usuário clicar.</t>
+  </si>
+  <si>
+    <t>Ao clicar para alugar sem estar com sessão iniciada, será redirecionado para a tela de login</t>
+  </si>
+  <si>
+    <t>Permitindo que qualquer prazo seja inserido para o aluguel</t>
+  </si>
+  <si>
+    <t>Encontre-nos</t>
+  </si>
+  <si>
+    <t>Localizar no mapa a locadora de veículos</t>
+  </si>
+  <si>
+    <t>CT-a006</t>
+  </si>
+  <si>
+    <t>Comprovante de aluguel para impressão após alugar veículo</t>
+  </si>
+  <si>
+    <t>Ter sessão iniciada no sistema, e ter algum disponível no sistema para realizar o aluguel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Executar o CT-a001 </t>
+  </si>
+  <si>
+    <t>Tela deve exibir o comprovante de aluguél para ser impresso e poder retirar o veículo</t>
+  </si>
+  <si>
+    <t>Tela só exibe a mensagem de veículo alugado, mas comprovante não é disponibilizado</t>
+  </si>
+  <si>
+    <t>CT-l001</t>
+  </si>
+  <si>
+    <t>Encontrar locadora</t>
+  </si>
+  <si>
+    <t>Acessar a opção 'Encontre-nos' no menu principal do sistema</t>
+  </si>
+  <si>
+    <t>Tela exibindo no mapa a localização da locadora de veículo</t>
+  </si>
+  <si>
+    <t>Mapa exibindo corretamente a localização da locadora de veículos</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -667,7 +726,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="14">
+  <fills count="15">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -744,6 +803,12 @@
       <patternFill patternType="solid">
         <fgColor theme="9"/>
         <bgColor rgb="FF339966"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor rgb="FF993300"/>
       </patternFill>
     </fill>
   </fills>
@@ -958,7 +1023,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="86">
+  <cellXfs count="89">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1147,6 +1212,12 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1170,6 +1241,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="14" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1287,7 +1361,7 @@
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
   <a:themeElements>
-    <a:clrScheme name="Escritório">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1325,7 +1399,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Escritório">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1397,7 +1471,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Escritório">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1550,7 +1624,7 @@
   <dimension ref="B3:J35"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E23" activeCellId="1" sqref="A6:XFD6 E23"/>
+      <selection activeCell="E23" activeCellId="1" sqref="A6:XFD6 E23:G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1674,11 +1748,11 @@
       <c r="B13" s="4"/>
       <c r="C13" s="5"/>
       <c r="D13" s="10"/>
-      <c r="E13" s="78" t="s">
+      <c r="E13" s="80" t="s">
         <v>0</v>
       </c>
-      <c r="F13" s="78"/>
-      <c r="G13" s="78"/>
+      <c r="F13" s="80"/>
+      <c r="G13" s="80"/>
       <c r="H13" s="11"/>
       <c r="I13" s="5"/>
       <c r="J13" s="6"/>
@@ -1687,9 +1761,9 @@
       <c r="B14" s="4"/>
       <c r="C14" s="5"/>
       <c r="D14" s="10"/>
-      <c r="E14" s="78"/>
-      <c r="F14" s="78"/>
-      <c r="G14" s="78"/>
+      <c r="E14" s="80"/>
+      <c r="F14" s="80"/>
+      <c r="G14" s="80"/>
       <c r="H14" s="11"/>
       <c r="I14" s="5"/>
       <c r="J14" s="6"/>
@@ -1709,11 +1783,11 @@
       <c r="B16" s="4"/>
       <c r="C16" s="5"/>
       <c r="D16" s="10"/>
-      <c r="E16" s="79" t="s">
+      <c r="E16" s="81" t="s">
         <v>1</v>
       </c>
-      <c r="F16" s="79"/>
-      <c r="G16" s="79"/>
+      <c r="F16" s="81"/>
+      <c r="G16" s="81"/>
       <c r="H16" s="11"/>
       <c r="I16" s="5"/>
       <c r="J16" s="6"/>
@@ -1722,9 +1796,9 @@
       <c r="B17" s="4"/>
       <c r="C17" s="5"/>
       <c r="D17" s="10"/>
-      <c r="E17" s="79"/>
-      <c r="F17" s="79"/>
-      <c r="G17" s="79"/>
+      <c r="E17" s="81"/>
+      <c r="F17" s="81"/>
+      <c r="G17" s="81"/>
       <c r="H17" s="11"/>
       <c r="I17" s="5"/>
       <c r="J17" s="6"/>
@@ -1770,11 +1844,11 @@
       <c r="B21" s="4"/>
       <c r="C21" s="5"/>
       <c r="D21" s="10"/>
-      <c r="E21" s="80" t="s">
+      <c r="E21" s="82" t="s">
         <v>4</v>
       </c>
-      <c r="F21" s="80"/>
-      <c r="G21" s="80"/>
+      <c r="F21" s="82"/>
+      <c r="G21" s="82"/>
       <c r="H21" s="11"/>
       <c r="I21" s="5"/>
       <c r="J21" s="6"/>
@@ -1783,11 +1857,11 @@
       <c r="B22" s="4"/>
       <c r="C22" s="5"/>
       <c r="D22" s="10"/>
-      <c r="E22" s="80" t="s">
+      <c r="E22" s="82" t="s">
         <v>5</v>
       </c>
-      <c r="F22" s="80"/>
-      <c r="G22" s="80"/>
+      <c r="F22" s="82"/>
+      <c r="G22" s="82"/>
       <c r="H22" s="11"/>
       <c r="I22" s="5"/>
       <c r="J22" s="6"/>
@@ -1796,9 +1870,9 @@
       <c r="B23" s="4"/>
       <c r="C23" s="5"/>
       <c r="D23" s="10"/>
-      <c r="E23" s="81"/>
-      <c r="F23" s="81"/>
-      <c r="G23" s="81"/>
+      <c r="E23" s="83"/>
+      <c r="F23" s="83"/>
+      <c r="G23" s="83"/>
       <c r="H23" s="11"/>
       <c r="I23" s="5"/>
       <c r="J23" s="6"/>
@@ -1952,8 +2026,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L24" activeCellId="1" sqref="A6:XFD6 L24"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1970,8 +2044,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G76"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:XFD6"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2026,11 +2100,11 @@
       <c r="A3" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="82" t="s">
+      <c r="B3" s="84" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="82"/>
-      <c r="D3" s="82"/>
+      <c r="C3" s="84"/>
+      <c r="D3" s="84"/>
       <c r="E3" s="34"/>
       <c r="F3" s="35"/>
       <c r="G3" s="33"/>
@@ -2080,10 +2154,10 @@
         <v>25</v>
       </c>
       <c r="F6" s="47" t="s">
-        <v>26</v>
-      </c>
-      <c r="G6" s="48" t="s">
-        <v>27</v>
+        <v>183</v>
+      </c>
+      <c r="G6" s="88" t="s">
+        <v>182</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
@@ -2097,10 +2171,10 @@
     </row>
     <row r="8" spans="1:7" ht="51" x14ac:dyDescent="0.2">
       <c r="A8" s="44" t="s">
+        <v>27</v>
+      </c>
+      <c r="B8" s="45" t="s">
         <v>28</v>
-      </c>
-      <c r="B8" s="45" t="s">
-        <v>29</v>
       </c>
       <c r="C8" s="45" t="s">
         <v>23</v>
@@ -2109,13 +2183,13 @@
         <v>24</v>
       </c>
       <c r="E8" s="46" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F8" s="47" t="s">
-        <v>26</v>
+        <v>183</v>
       </c>
       <c r="G8" s="48" t="s">
-        <v>27</v>
+        <v>184</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
@@ -2127,27 +2201,27 @@
       <c r="F9" s="50"/>
       <c r="G9" s="50"/>
     </row>
-    <row r="10" spans="1:7" ht="51" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A10" s="44" t="s">
+        <v>30</v>
+      </c>
+      <c r="B10" s="45" t="s">
         <v>31</v>
-      </c>
-      <c r="B10" s="45" t="s">
-        <v>32</v>
       </c>
       <c r="C10" s="45" t="s">
         <v>23</v>
       </c>
       <c r="D10" s="45" t="s">
-        <v>24</v>
+        <v>185</v>
       </c>
       <c r="E10" s="46" t="s">
-        <v>33</v>
+        <v>186</v>
       </c>
       <c r="F10" s="47" t="s">
-        <v>26</v>
-      </c>
-      <c r="G10" s="48" t="s">
-        <v>27</v>
+        <v>183</v>
+      </c>
+      <c r="G10" s="88" t="s">
+        <v>187</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
@@ -2161,25 +2235,25 @@
     </row>
     <row r="12" spans="1:7" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A12" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="B12" s="45" t="s">
+        <v>33</v>
+      </c>
+      <c r="C12" s="45" t="s">
+        <v>26</v>
+      </c>
+      <c r="D12" s="45" t="s">
         <v>34</v>
       </c>
-      <c r="B12" s="45" t="s">
+      <c r="E12" s="46" t="s">
         <v>35</v>
       </c>
-      <c r="C12" s="45" t="s">
-        <v>27</v>
-      </c>
-      <c r="D12" s="45" t="s">
-        <v>36</v>
-      </c>
-      <c r="E12" s="46" t="s">
-        <v>37</v>
-      </c>
       <c r="F12" s="47" t="s">
-        <v>27</v>
-      </c>
-      <c r="G12" s="48" t="s">
-        <v>27</v>
+        <v>26</v>
+      </c>
+      <c r="G12" s="88" t="s">
+        <v>188</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
@@ -2193,25 +2267,25 @@
     </row>
     <row r="14" spans="1:7" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A14" s="44" t="s">
+        <v>36</v>
+      </c>
+      <c r="B14" s="45" t="s">
+        <v>37</v>
+      </c>
+      <c r="C14" s="45" t="s">
         <v>38</v>
       </c>
-      <c r="B14" s="45" t="s">
+      <c r="D14" s="45" t="s">
         <v>39</v>
       </c>
-      <c r="C14" s="45" t="s">
+      <c r="E14" s="46" t="s">
         <v>40</v>
       </c>
-      <c r="D14" s="45" t="s">
+      <c r="F14" s="47" t="s">
         <v>41</v>
       </c>
-      <c r="E14" s="46" t="s">
-        <v>42</v>
-      </c>
-      <c r="F14" s="47" t="s">
-        <v>43</v>
-      </c>
       <c r="G14" s="48" t="s">
-        <v>27</v>
+        <v>189</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
@@ -2224,13 +2298,27 @@
       <c r="G15" s="50"/>
     </row>
     <row r="16" spans="1:7" ht="56.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="44"/>
-      <c r="B16" s="45"/>
-      <c r="C16" s="45"/>
-      <c r="D16" s="45"/>
-      <c r="E16" s="46"/>
-      <c r="F16" s="52"/>
-      <c r="G16" s="53"/>
+      <c r="A16" s="44" t="s">
+        <v>192</v>
+      </c>
+      <c r="B16" s="45" t="s">
+        <v>193</v>
+      </c>
+      <c r="C16" s="45" t="s">
+        <v>194</v>
+      </c>
+      <c r="D16" s="45" t="s">
+        <v>195</v>
+      </c>
+      <c r="E16" s="46" t="s">
+        <v>196</v>
+      </c>
+      <c r="F16" s="47" t="s">
+        <v>183</v>
+      </c>
+      <c r="G16" s="48" t="s">
+        <v>197</v>
+      </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" s="49"/>
@@ -2333,7 +2421,7 @@
     </row>
     <row r="28" spans="1:7" ht="65.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="44" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B28" s="55"/>
       <c r="C28" s="55"/>
@@ -2353,7 +2441,7 @@
     </row>
     <row r="30" spans="1:7" ht="58.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="44" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B30" s="45"/>
       <c r="C30" s="45"/>
@@ -2373,7 +2461,7 @@
     </row>
     <row r="32" spans="1:7" ht="56.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="44" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B32" s="45"/>
       <c r="C32" s="55"/>
@@ -2393,7 +2481,7 @@
     </row>
     <row r="34" spans="1:7" ht="69" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="44" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B34" s="45"/>
       <c r="C34" s="45"/>
@@ -2413,7 +2501,7 @@
     </row>
     <row r="36" spans="1:7" ht="58.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="44" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B36" s="45"/>
       <c r="C36" s="45"/>
@@ -2433,7 +2521,7 @@
     </row>
     <row r="38" spans="1:7" ht="54" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="44" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B38" s="45"/>
       <c r="C38" s="45"/>
@@ -2453,7 +2541,7 @@
     </row>
     <row r="40" spans="1:7" ht="63.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="44" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B40" s="45"/>
       <c r="C40" s="45"/>
@@ -2473,7 +2561,7 @@
     </row>
     <row r="42" spans="1:7" ht="61.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="44" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B42" s="45"/>
       <c r="C42" s="45"/>
@@ -2493,7 +2581,7 @@
     </row>
     <row r="44" spans="1:7" ht="64.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="44" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B44" s="45"/>
       <c r="C44" s="45"/>
@@ -2513,7 +2601,7 @@
     </row>
     <row r="46" spans="1:7" ht="57.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="44" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B46" s="55"/>
       <c r="C46" s="55"/>
@@ -2527,7 +2615,7 @@
     </row>
     <row r="48" spans="1:7" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="44" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B48" s="55"/>
       <c r="C48" s="55"/>
@@ -2541,7 +2629,7 @@
     </row>
     <row r="50" spans="1:7" ht="58.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="44" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B50" s="55"/>
       <c r="C50" s="55"/>
@@ -2555,7 +2643,7 @@
     </row>
     <row r="52" spans="1:7" ht="55.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="44" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B52" s="55"/>
       <c r="C52" s="55"/>
@@ -2569,7 +2657,7 @@
     </row>
     <row r="54" spans="1:7" ht="55.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="44" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B54" s="45"/>
       <c r="C54" s="45"/>
@@ -2583,7 +2671,7 @@
     </row>
     <row r="56" spans="1:7" ht="51.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="44" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B56" s="45"/>
       <c r="C56" s="45"/>
@@ -2597,7 +2685,7 @@
     </row>
     <row r="58" spans="1:7" ht="52.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" s="44" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B58" s="45"/>
       <c r="C58" s="45"/>
@@ -2611,7 +2699,7 @@
     </row>
     <row r="60" spans="1:7" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" s="44" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B60" s="45"/>
       <c r="C60" s="45"/>
@@ -2622,7 +2710,7 @@
     </row>
     <row r="62" spans="1:7" ht="54.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A62" s="44" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B62" s="45"/>
       <c r="C62" s="45"/>
@@ -2636,7 +2724,7 @@
     </row>
     <row r="64" spans="1:7" ht="56.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64" s="44" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B64" s="45"/>
       <c r="C64" s="45"/>
@@ -2650,7 +2738,7 @@
     </row>
     <row r="66" spans="1:7" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A66" s="44" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B66" s="45"/>
       <c r="C66" s="45"/>
@@ -2724,9 +2812,10 @@
     <mergeCell ref="B3:D3"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="F6" r:id="rId1"/>
-    <hyperlink ref="F8" r:id="rId2"/>
-    <hyperlink ref="F10" r:id="rId3"/>
+    <hyperlink ref="F6" r:id="rId1" display="LOGIN: cimara@gmail.com_x000a_SENHA: 1234"/>
+    <hyperlink ref="F8" r:id="rId2" display="LOGIN: cimara@gmail.com_x000a_SENHA: 1234"/>
+    <hyperlink ref="F10" r:id="rId3" display="LOGIN: cimara@gmail.com_x000a_SENHA: 1234"/>
+    <hyperlink ref="F16" r:id="rId4" display="LOGIN: cimara@gmail.com_x000a_SENHA: 1234"/>
   </hyperlinks>
   <pageMargins left="0.51180555555555496" right="0.51180555555555496" top="0.78749999999999998" bottom="0.78749999999999998" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
@@ -2737,8 +2826,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G38"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F10" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2779,7 +2868,7 @@
         <v>10</v>
       </c>
       <c r="B2" s="29" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C2" s="30"/>
       <c r="D2" s="31"/>
@@ -2793,11 +2882,11 @@
       <c r="A3" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="82" t="s">
-        <v>65</v>
-      </c>
-      <c r="C3" s="82"/>
-      <c r="D3" s="82"/>
+      <c r="B3" s="84" t="s">
+        <v>63</v>
+      </c>
+      <c r="C3" s="84"/>
+      <c r="D3" s="84"/>
       <c r="E3" s="34"/>
       <c r="F3" s="35"/>
       <c r="G3" s="33"/>
@@ -2832,25 +2921,25 @@
     </row>
     <row r="6" spans="1:7" ht="45.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="44" t="s">
+        <v>64</v>
+      </c>
+      <c r="B6" s="45" t="s">
+        <v>65</v>
+      </c>
+      <c r="C6" s="45" t="s">
         <v>66</v>
       </c>
-      <c r="B6" s="45" t="s">
+      <c r="D6" s="45" t="s">
         <v>67</v>
       </c>
-      <c r="C6" s="45" t="s">
+      <c r="E6" s="46" t="s">
         <v>68</v>
       </c>
-      <c r="D6" s="45" t="s">
+      <c r="F6" s="47" t="s">
         <v>69</v>
       </c>
-      <c r="E6" s="46" t="s">
+      <c r="G6" s="75" t="s">
         <v>70</v>
-      </c>
-      <c r="F6" s="47" t="s">
-        <v>71</v>
-      </c>
-      <c r="G6" s="75" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
@@ -2864,25 +2953,25 @@
     </row>
     <row r="8" spans="1:7" ht="51" x14ac:dyDescent="0.2">
       <c r="A8" s="44" t="s">
+        <v>71</v>
+      </c>
+      <c r="B8" s="45" t="s">
+        <v>72</v>
+      </c>
+      <c r="C8" s="44" t="s">
+        <v>26</v>
+      </c>
+      <c r="D8" s="45" t="s">
         <v>73</v>
       </c>
-      <c r="B8" s="45" t="s">
+      <c r="E8" s="46" t="s">
         <v>74</v>
       </c>
-      <c r="C8" s="44" t="s">
-        <v>27</v>
-      </c>
-      <c r="D8" s="45" t="s">
+      <c r="F8" s="47" t="s">
         <v>75</v>
       </c>
-      <c r="E8" s="46" t="s">
+      <c r="G8" s="75" t="s">
         <v>76</v>
-      </c>
-      <c r="F8" s="47" t="s">
-        <v>77</v>
-      </c>
-      <c r="G8" s="75" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
@@ -2896,25 +2985,25 @@
     </row>
     <row r="10" spans="1:7" ht="54" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="44" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B10" s="44" t="s">
+        <v>137</v>
+      </c>
+      <c r="C10" s="44" t="s">
+        <v>138</v>
+      </c>
+      <c r="D10" s="44" t="s">
         <v>139</v>
       </c>
-      <c r="C10" s="44" t="s">
+      <c r="E10" s="72" t="s">
         <v>140</v>
       </c>
-      <c r="D10" s="44" t="s">
-        <v>141</v>
-      </c>
-      <c r="E10" s="72" t="s">
-        <v>142</v>
-      </c>
       <c r="F10" s="73" t="s">
+        <v>138</v>
+      </c>
+      <c r="G10" s="74" t="s">
         <v>140</v>
-      </c>
-      <c r="G10" s="74" t="s">
-        <v>142</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
@@ -3162,7 +3251,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G24"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
@@ -3204,7 +3293,7 @@
         <v>10</v>
       </c>
       <c r="B2" s="29" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C2" s="30"/>
       <c r="D2" s="31"/>
@@ -3218,11 +3307,11 @@
       <c r="A3" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="83" t="s">
-        <v>80</v>
-      </c>
-      <c r="C3" s="83"/>
-      <c r="D3" s="83"/>
+      <c r="B3" s="85" t="s">
+        <v>78</v>
+      </c>
+      <c r="C3" s="85"/>
+      <c r="D3" s="85"/>
       <c r="E3" s="34"/>
       <c r="F3" s="35"/>
       <c r="G3" s="66"/>
@@ -3257,25 +3346,25 @@
     </row>
     <row r="6" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A6" s="44" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B6" s="45" t="s">
+        <v>80</v>
+      </c>
+      <c r="C6" s="71" t="s">
+        <v>138</v>
+      </c>
+      <c r="D6" s="45" t="s">
         <v>82</v>
       </c>
-      <c r="C6" s="71" t="s">
-        <v>140</v>
-      </c>
-      <c r="D6" s="45" t="s">
+      <c r="E6" s="46" t="s">
+        <v>83</v>
+      </c>
+      <c r="F6" s="47" t="s">
         <v>84</v>
       </c>
-      <c r="E6" s="46" t="s">
+      <c r="G6" s="64" t="s">
         <v>85</v>
-      </c>
-      <c r="F6" s="47" t="s">
-        <v>86</v>
-      </c>
-      <c r="G6" s="64" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
@@ -3289,25 +3378,25 @@
     </row>
     <row r="8" spans="1:7" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A8" s="44" t="s">
+        <v>86</v>
+      </c>
+      <c r="B8" s="45" t="s">
+        <v>87</v>
+      </c>
+      <c r="C8" s="45" t="s">
         <v>88</v>
       </c>
-      <c r="B8" s="45" t="s">
+      <c r="D8" s="45" t="s">
         <v>89</v>
       </c>
-      <c r="C8" s="45" t="s">
+      <c r="E8" s="46" t="s">
         <v>90</v>
       </c>
-      <c r="D8" s="45" t="s">
+      <c r="F8" s="47" t="s">
+        <v>84</v>
+      </c>
+      <c r="G8" s="48" t="s">
         <v>91</v>
-      </c>
-      <c r="E8" s="46" t="s">
-        <v>92</v>
-      </c>
-      <c r="F8" s="47" t="s">
-        <v>86</v>
-      </c>
-      <c r="G8" s="48" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
@@ -3321,25 +3410,25 @@
     </row>
     <row r="10" spans="1:7" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A10" s="44" t="s">
+        <v>92</v>
+      </c>
+      <c r="B10" s="45" t="s">
+        <v>93</v>
+      </c>
+      <c r="C10" s="45" t="s">
         <v>94</v>
       </c>
-      <c r="B10" s="45" t="s">
+      <c r="D10" s="45" t="s">
         <v>95</v>
       </c>
-      <c r="C10" s="45" t="s">
-        <v>96</v>
-      </c>
-      <c r="D10" s="45" t="s">
-        <v>97</v>
-      </c>
       <c r="E10" s="46" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="F10" s="47" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="G10" s="64" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
@@ -3353,25 +3442,25 @@
     </row>
     <row r="12" spans="1:7" ht="51" x14ac:dyDescent="0.2">
       <c r="A12" s="44" t="s">
+        <v>96</v>
+      </c>
+      <c r="B12" s="45" t="s">
+        <v>97</v>
+      </c>
+      <c r="C12" s="45" t="s">
+        <v>81</v>
+      </c>
+      <c r="D12" s="45" t="s">
         <v>98</v>
       </c>
-      <c r="B12" s="45" t="s">
+      <c r="E12" s="46" t="s">
         <v>99</v>
       </c>
-      <c r="C12" s="45" t="s">
-        <v>83</v>
-      </c>
-      <c r="D12" s="45" t="s">
+      <c r="F12" s="47" t="s">
         <v>100</v>
       </c>
-      <c r="E12" s="46" t="s">
-        <v>101</v>
-      </c>
-      <c r="F12" s="47" t="s">
-        <v>102</v>
-      </c>
       <c r="G12" s="64" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
@@ -3385,25 +3474,25 @@
     </row>
     <row r="14" spans="1:7" ht="51" x14ac:dyDescent="0.2">
       <c r="A14" s="71" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="B14" s="71" t="s">
+        <v>142</v>
+      </c>
+      <c r="C14" s="71" t="s">
+        <v>138</v>
+      </c>
+      <c r="D14" s="71" t="s">
+        <v>143</v>
+      </c>
+      <c r="E14" s="72" t="s">
         <v>144</v>
       </c>
-      <c r="C14" s="71" t="s">
-        <v>140</v>
-      </c>
-      <c r="D14" s="71" t="s">
-        <v>145</v>
-      </c>
-      <c r="E14" s="72" t="s">
-        <v>146</v>
-      </c>
       <c r="F14" s="73" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="G14" s="74" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
@@ -3417,25 +3506,25 @@
     </row>
     <row r="16" spans="1:7" ht="51" x14ac:dyDescent="0.2">
       <c r="A16" s="71" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="B16" s="71" t="s">
+        <v>145</v>
+      </c>
+      <c r="C16" s="71" t="s">
+        <v>138</v>
+      </c>
+      <c r="D16" s="71" t="s">
+        <v>146</v>
+      </c>
+      <c r="E16" s="72" t="s">
         <v>147</v>
       </c>
-      <c r="C16" s="71" t="s">
-        <v>140</v>
-      </c>
-      <c r="D16" s="71" t="s">
-        <v>148</v>
-      </c>
-      <c r="E16" s="72" t="s">
-        <v>149</v>
-      </c>
       <c r="F16" s="73" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="G16" s="74" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
@@ -3449,25 +3538,25 @@
     </row>
     <row r="18" spans="1:7" ht="51" x14ac:dyDescent="0.2">
       <c r="A18" s="71" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B18" s="71" t="s">
+        <v>148</v>
+      </c>
+      <c r="C18" s="71" t="s">
+        <v>138</v>
+      </c>
+      <c r="D18" s="71" t="s">
+        <v>149</v>
+      </c>
+      <c r="E18" s="72" t="s">
         <v>150</v>
       </c>
-      <c r="C18" s="71" t="s">
-        <v>140</v>
-      </c>
-      <c r="D18" s="71" t="s">
-        <v>151</v>
-      </c>
-      <c r="E18" s="72" t="s">
-        <v>152</v>
-      </c>
       <c r="F18" s="73" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="G18" s="74" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
@@ -3481,25 +3570,25 @@
     </row>
     <row r="20" spans="1:7" ht="51" x14ac:dyDescent="0.2">
       <c r="A20" s="71" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B20" s="71" t="s">
+        <v>151</v>
+      </c>
+      <c r="C20" s="71" t="s">
+        <v>138</v>
+      </c>
+      <c r="D20" s="71" t="s">
+        <v>152</v>
+      </c>
+      <c r="E20" s="72" t="s">
         <v>153</v>
       </c>
-      <c r="C20" s="71" t="s">
-        <v>140</v>
-      </c>
-      <c r="D20" s="71" t="s">
-        <v>154</v>
-      </c>
-      <c r="E20" s="72" t="s">
-        <v>155</v>
-      </c>
       <c r="F20" s="73" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="G20" s="74" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
@@ -3513,25 +3602,25 @@
     </row>
     <row r="22" spans="1:7" ht="51" x14ac:dyDescent="0.2">
       <c r="A22" s="71" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="B22" s="71" t="s">
+        <v>154</v>
+      </c>
+      <c r="C22" s="71" t="s">
+        <v>138</v>
+      </c>
+      <c r="D22" s="71" t="s">
+        <v>155</v>
+      </c>
+      <c r="E22" s="72" t="s">
         <v>156</v>
       </c>
-      <c r="C22" s="71" t="s">
-        <v>140</v>
-      </c>
-      <c r="D22" s="71" t="s">
-        <v>157</v>
-      </c>
-      <c r="E22" s="72" t="s">
-        <v>158</v>
-      </c>
       <c r="F22" s="73" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="G22" s="74" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
@@ -3545,25 +3634,25 @@
     </row>
     <row r="24" spans="1:7" ht="63.75" x14ac:dyDescent="0.2">
       <c r="A24" s="71" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="B24" s="71" t="s">
+        <v>157</v>
+      </c>
+      <c r="C24" s="71" t="s">
+        <v>138</v>
+      </c>
+      <c r="D24" s="71" t="s">
+        <v>158</v>
+      </c>
+      <c r="E24" s="72" t="s">
         <v>159</v>
       </c>
-      <c r="C24" s="71" t="s">
-        <v>140</v>
-      </c>
-      <c r="D24" s="71" t="s">
+      <c r="F24" s="73" t="s">
         <v>160</v>
       </c>
-      <c r="E24" s="72" t="s">
-        <v>161</v>
-      </c>
-      <c r="F24" s="73" t="s">
-        <v>162</v>
-      </c>
       <c r="G24" s="74" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
   </sheetData>
@@ -3579,7 +3668,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
@@ -3621,7 +3710,7 @@
         <v>10</v>
       </c>
       <c r="B2" s="29" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C2" s="30"/>
       <c r="D2" s="31"/>
@@ -3635,11 +3724,11 @@
       <c r="A3" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="84" t="s">
-        <v>104</v>
-      </c>
-      <c r="C3" s="84"/>
-      <c r="D3" s="84"/>
+      <c r="B3" s="86" t="s">
+        <v>102</v>
+      </c>
+      <c r="C3" s="86"/>
+      <c r="D3" s="86"/>
       <c r="E3" s="34"/>
       <c r="F3" s="35"/>
       <c r="G3" s="66"/>
@@ -3674,25 +3763,25 @@
     </row>
     <row r="6" spans="1:7" ht="36.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="44" t="s">
+        <v>79</v>
+      </c>
+      <c r="B6" s="45" t="s">
+        <v>103</v>
+      </c>
+      <c r="C6" s="45" t="s">
         <v>81</v>
       </c>
-      <c r="B6" s="45" t="s">
-        <v>105</v>
-      </c>
-      <c r="C6" s="45" t="s">
+      <c r="D6" s="45" t="s">
+        <v>82</v>
+      </c>
+      <c r="E6" s="46" t="s">
         <v>83</v>
       </c>
-      <c r="D6" s="45" t="s">
+      <c r="F6" s="47" t="s">
         <v>84</v>
       </c>
-      <c r="E6" s="46" t="s">
+      <c r="G6" s="64" t="s">
         <v>85</v>
-      </c>
-      <c r="F6" s="47" t="s">
-        <v>86</v>
-      </c>
-      <c r="G6" s="64" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
@@ -3706,25 +3795,25 @@
     </row>
     <row r="8" spans="1:7" ht="51" x14ac:dyDescent="0.2">
       <c r="A8" s="44" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B8" s="45" t="s">
+        <v>104</v>
+      </c>
+      <c r="C8" s="45" t="s">
+        <v>105</v>
+      </c>
+      <c r="D8" s="45" t="s">
         <v>106</v>
       </c>
-      <c r="C8" s="45" t="s">
-        <v>107</v>
-      </c>
-      <c r="D8" s="45" t="s">
-        <v>108</v>
-      </c>
       <c r="E8" s="46" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="F8" s="47" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="G8" s="48" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
@@ -3738,25 +3827,25 @@
     </row>
     <row r="10" spans="1:7" ht="51" x14ac:dyDescent="0.2">
       <c r="A10" s="44" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B10" s="45" t="s">
+        <v>107</v>
+      </c>
+      <c r="C10" s="45" t="s">
+        <v>108</v>
+      </c>
+      <c r="D10" s="45" t="s">
         <v>109</v>
       </c>
-      <c r="C10" s="45" t="s">
-        <v>110</v>
-      </c>
-      <c r="D10" s="45" t="s">
-        <v>111</v>
-      </c>
       <c r="E10" s="46" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="F10" s="47" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="G10" s="64" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
@@ -3770,25 +3859,25 @@
     </row>
     <row r="12" spans="1:7" ht="51" x14ac:dyDescent="0.2">
       <c r="A12" s="44" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B12" s="45" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C12" s="45" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D12" s="45" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="E12" s="46" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="F12" s="47" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="G12" s="64" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
@@ -3802,25 +3891,25 @@
     </row>
     <row r="14" spans="1:7" ht="76.5" x14ac:dyDescent="0.2">
       <c r="A14" s="76" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="B14" s="76" t="s">
+        <v>167</v>
+      </c>
+      <c r="C14" s="76" t="s">
+        <v>138</v>
+      </c>
+      <c r="D14" s="76" t="s">
+        <v>168</v>
+      </c>
+      <c r="E14" s="72" t="s">
         <v>169</v>
       </c>
-      <c r="C14" s="76" t="s">
-        <v>140</v>
-      </c>
-      <c r="D14" s="76" t="s">
-        <v>170</v>
-      </c>
-      <c r="E14" s="72" t="s">
-        <v>171</v>
-      </c>
       <c r="F14" s="73" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="G14" s="74" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
@@ -3834,25 +3923,25 @@
     </row>
     <row r="16" spans="1:7" ht="89.25" x14ac:dyDescent="0.2">
       <c r="A16" s="76" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="B16" s="76" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="C16" s="76" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="D16" s="76" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="E16" s="72" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="F16" s="73" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="G16" s="74" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
@@ -3866,25 +3955,25 @@
     </row>
     <row r="18" spans="1:7" ht="89.25" x14ac:dyDescent="0.2">
       <c r="A18" s="76" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B18" s="76" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="C18" s="76" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="D18" s="76" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="E18" s="72" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="F18" s="73" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="G18" s="74" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
@@ -3898,25 +3987,25 @@
     </row>
     <row r="20" spans="1:7" ht="51" x14ac:dyDescent="0.2">
       <c r="A20" s="76" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B20" s="76" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="C20" s="76" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="D20" s="76" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="E20" s="72" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="F20" s="73" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="G20" s="74" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
@@ -3930,25 +4019,25 @@
     </row>
     <row r="22" spans="1:7" ht="89.25" x14ac:dyDescent="0.2">
       <c r="A22" s="76" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="B22" s="76" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="C22" s="76" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="D22" s="76" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="E22" s="72" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="F22" s="73" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="G22" s="74" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
@@ -3962,25 +4051,25 @@
     </row>
     <row r="24" spans="1:7" ht="89.25" x14ac:dyDescent="0.2">
       <c r="A24" s="76" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="B24" s="76" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="C24" s="76" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="D24" s="76" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="E24" s="72" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="F24" s="73" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="G24" s="74" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.2">
@@ -3994,25 +4083,25 @@
     </row>
     <row r="26" spans="1:7" ht="89.25" x14ac:dyDescent="0.2">
       <c r="A26" s="76" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="B26" s="76" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="C26" s="76" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="D26" s="76" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="E26" s="72" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="F26" s="73" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="G26" s="74" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
   </sheetData>
@@ -4028,7 +4117,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G56"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
@@ -4070,7 +4159,7 @@
         <v>10</v>
       </c>
       <c r="B2" s="29" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C2" s="30"/>
       <c r="D2" s="31"/>
@@ -4084,11 +4173,11 @@
       <c r="A3" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="85" t="s">
-        <v>104</v>
-      </c>
-      <c r="C3" s="85"/>
-      <c r="D3" s="85"/>
+      <c r="B3" s="87" t="s">
+        <v>102</v>
+      </c>
+      <c r="C3" s="87"/>
+      <c r="D3" s="87"/>
       <c r="E3" s="34"/>
       <c r="F3" s="35"/>
       <c r="G3" s="66"/>
@@ -4123,25 +4212,25 @@
     </row>
     <row r="6" spans="1:7" ht="97.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="44" t="s">
+        <v>113</v>
+      </c>
+      <c r="B6" s="45" t="s">
+        <v>114</v>
+      </c>
+      <c r="C6" s="45" t="s">
         <v>115</v>
       </c>
-      <c r="B6" s="45" t="s">
+      <c r="D6" s="45" t="s">
         <v>116</v>
       </c>
-      <c r="C6" s="45" t="s">
+      <c r="E6" s="46" t="s">
+        <v>85</v>
+      </c>
+      <c r="F6" s="47" t="s">
         <v>117</v>
       </c>
-      <c r="D6" s="45" t="s">
-        <v>118</v>
-      </c>
-      <c r="E6" s="46" t="s">
-        <v>87</v>
-      </c>
-      <c r="F6" s="47" t="s">
-        <v>119</v>
-      </c>
       <c r="G6" s="64" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
@@ -4155,25 +4244,25 @@
     </row>
     <row r="8" spans="1:7" ht="97.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="44" t="s">
+        <v>118</v>
+      </c>
+      <c r="B8" s="45" t="s">
+        <v>119</v>
+      </c>
+      <c r="C8" s="45" t="s">
+        <v>115</v>
+      </c>
+      <c r="D8" s="45" t="s">
         <v>120</v>
       </c>
-      <c r="B8" s="45" t="s">
+      <c r="E8" s="46" t="s">
         <v>121</v>
       </c>
-      <c r="C8" s="45" t="s">
+      <c r="F8" s="47" t="s">
         <v>117</v>
       </c>
-      <c r="D8" s="45" t="s">
-        <v>122</v>
-      </c>
-      <c r="E8" s="46" t="s">
-        <v>123</v>
-      </c>
-      <c r="F8" s="47" t="s">
-        <v>119</v>
-      </c>
       <c r="G8" s="64" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
@@ -4187,25 +4276,25 @@
     </row>
     <row r="10" spans="1:7" ht="72.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="44" t="s">
+        <v>122</v>
+      </c>
+      <c r="B10" s="45" t="s">
+        <v>123</v>
+      </c>
+      <c r="C10" s="45" t="s">
+        <v>115</v>
+      </c>
+      <c r="D10" s="45" t="s">
+        <v>116</v>
+      </c>
+      <c r="E10" s="46" t="s">
         <v>124</v>
       </c>
-      <c r="B10" s="45" t="s">
+      <c r="F10" s="47" t="s">
         <v>125</v>
       </c>
-      <c r="C10" s="45" t="s">
-        <v>117</v>
-      </c>
-      <c r="D10" s="45" t="s">
-        <v>118</v>
-      </c>
-      <c r="E10" s="46" t="s">
+      <c r="G10" s="48" t="s">
         <v>126</v>
-      </c>
-      <c r="F10" s="47" t="s">
-        <v>127</v>
-      </c>
-      <c r="G10" s="48" t="s">
-        <v>128</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
@@ -4219,25 +4308,25 @@
     </row>
     <row r="12" spans="1:7" ht="97.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="44" t="s">
+        <v>127</v>
+      </c>
+      <c r="B12" s="45" t="s">
+        <v>128</v>
+      </c>
+      <c r="C12" s="45" t="s">
         <v>129</v>
       </c>
-      <c r="B12" s="45" t="s">
+      <c r="D12" s="45" t="s">
         <v>130</v>
       </c>
-      <c r="C12" s="45" t="s">
+      <c r="E12" s="46" t="s">
         <v>131</v>
       </c>
-      <c r="D12" s="45" t="s">
+      <c r="F12" s="47" t="s">
         <v>132</v>
       </c>
-      <c r="E12" s="46" t="s">
-        <v>133</v>
-      </c>
-      <c r="F12" s="47" t="s">
-        <v>134</v>
-      </c>
       <c r="G12" s="64" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
@@ -4251,25 +4340,25 @@
     </row>
     <row r="14" spans="1:7" ht="97.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="44" t="s">
+        <v>133</v>
+      </c>
+      <c r="B14" s="45" t="s">
+        <v>134</v>
+      </c>
+      <c r="C14" s="45" t="s">
+        <v>129</v>
+      </c>
+      <c r="D14" s="45" t="s">
+        <v>130</v>
+      </c>
+      <c r="E14" s="46" t="s">
         <v>135</v>
       </c>
-      <c r="B14" s="45" t="s">
+      <c r="F14" s="47" t="s">
+        <v>132</v>
+      </c>
+      <c r="G14" s="48" t="s">
         <v>136</v>
-      </c>
-      <c r="C14" s="45" t="s">
-        <v>131</v>
-      </c>
-      <c r="D14" s="45" t="s">
-        <v>132</v>
-      </c>
-      <c r="E14" s="46" t="s">
-        <v>137</v>
-      </c>
-      <c r="F14" s="47" t="s">
-        <v>134</v>
-      </c>
-      <c r="G14" s="48" t="s">
-        <v>138</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
@@ -4627,4 +4716,394 @@
   <pageMargins left="0.51180555555555496" right="0.51180555555555496" top="0.78749999999999998" bottom="0.78749999999999998" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G38"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H1" sqref="H1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="17" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="31.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="25.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" s="28" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="22" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="24"/>
+      <c r="D1" s="25" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" s="25" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="26" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" s="27" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="29" t="s">
+        <v>190</v>
+      </c>
+      <c r="C2" s="30"/>
+      <c r="D2" s="31"/>
+      <c r="E2" s="25" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2" s="32"/>
+      <c r="G2" s="33"/>
+    </row>
+    <row r="3" spans="1:7" ht="34.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="22" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" s="84" t="s">
+        <v>191</v>
+      </c>
+      <c r="C3" s="84"/>
+      <c r="D3" s="84"/>
+      <c r="E3" s="34"/>
+      <c r="F3" s="35"/>
+      <c r="G3" s="33"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E4" s="36"/>
+      <c r="F4" s="37"/>
+      <c r="G4" s="38"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" s="39" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" s="40" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" s="39" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" s="39" t="s">
+        <v>18</v>
+      </c>
+      <c r="E5" s="41" t="s">
+        <v>19</v>
+      </c>
+      <c r="F5" s="42" t="s">
+        <v>20</v>
+      </c>
+      <c r="G5" s="43" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="51" x14ac:dyDescent="0.2">
+      <c r="A6" s="78" t="s">
+        <v>198</v>
+      </c>
+      <c r="B6" s="79" t="s">
+        <v>199</v>
+      </c>
+      <c r="C6" s="79" t="s">
+        <v>26</v>
+      </c>
+      <c r="D6" s="79" t="s">
+        <v>200</v>
+      </c>
+      <c r="E6" s="46" t="s">
+        <v>201</v>
+      </c>
+      <c r="F6" s="47" t="s">
+        <v>26</v>
+      </c>
+      <c r="G6" s="75" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7" s="49"/>
+      <c r="B7" s="50"/>
+      <c r="C7" s="50"/>
+      <c r="D7" s="50"/>
+      <c r="E7" s="50"/>
+      <c r="F7" s="50"/>
+      <c r="G7" s="50"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8" s="78"/>
+      <c r="B8" s="79"/>
+      <c r="C8" s="78"/>
+      <c r="D8" s="79"/>
+      <c r="E8" s="46"/>
+      <c r="F8" s="47"/>
+      <c r="G8" s="58"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9" s="54"/>
+      <c r="B9" s="50"/>
+      <c r="C9" s="50"/>
+      <c r="D9" s="50"/>
+      <c r="E9" s="50"/>
+      <c r="F9" s="50"/>
+    </row>
+    <row r="10" spans="1:7" ht="54" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="78"/>
+      <c r="B10" s="78"/>
+      <c r="C10" s="78"/>
+      <c r="D10" s="78"/>
+      <c r="E10" s="72"/>
+      <c r="F10" s="73"/>
+      <c r="G10" s="58"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11" s="59"/>
+      <c r="B11" s="60"/>
+      <c r="C11" s="50"/>
+      <c r="D11" s="50"/>
+      <c r="E11" s="50"/>
+      <c r="F11" s="50"/>
+      <c r="G11" s="50"/>
+    </row>
+    <row r="12" spans="1:7" ht="56.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="78"/>
+      <c r="B12" s="55"/>
+      <c r="C12" s="55"/>
+      <c r="D12" s="55"/>
+      <c r="E12" s="56"/>
+      <c r="F12" s="57"/>
+      <c r="G12" s="58"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A13" s="61"/>
+      <c r="B13" s="60"/>
+      <c r="C13" s="50"/>
+      <c r="D13" s="50"/>
+      <c r="E13" s="50"/>
+      <c r="F13" s="50"/>
+      <c r="G13" s="50"/>
+    </row>
+    <row r="14" spans="1:7" ht="62.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="78"/>
+      <c r="B14" s="55"/>
+      <c r="C14" s="55"/>
+      <c r="D14" s="55"/>
+      <c r="E14" s="56"/>
+      <c r="F14" s="57"/>
+      <c r="G14" s="58"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A15" s="61"/>
+      <c r="B15" s="60"/>
+      <c r="C15" s="50"/>
+      <c r="D15" s="50"/>
+      <c r="E15" s="50"/>
+      <c r="F15" s="50"/>
+      <c r="G15" s="50"/>
+    </row>
+    <row r="16" spans="1:7" ht="56.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="78"/>
+      <c r="B16" s="55"/>
+      <c r="C16" s="55"/>
+      <c r="D16" s="55"/>
+      <c r="E16" s="56"/>
+      <c r="F16" s="57"/>
+      <c r="G16" s="58"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A17" s="54"/>
+      <c r="B17" s="51"/>
+      <c r="C17" s="50"/>
+      <c r="D17" s="50"/>
+      <c r="E17" s="50"/>
+      <c r="F17" s="50"/>
+      <c r="G17" s="50"/>
+    </row>
+    <row r="18" spans="1:7" ht="65.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="78"/>
+      <c r="B18" s="55"/>
+      <c r="C18" s="55"/>
+      <c r="D18" s="55"/>
+      <c r="E18" s="56"/>
+      <c r="F18" s="57"/>
+      <c r="G18" s="58"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A19" s="54"/>
+      <c r="B19" s="50"/>
+      <c r="C19" s="50"/>
+      <c r="D19" s="50"/>
+      <c r="E19" s="50"/>
+      <c r="F19" s="50"/>
+      <c r="G19" s="50"/>
+    </row>
+    <row r="20" spans="1:7" ht="58.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="78"/>
+      <c r="B20" s="79"/>
+      <c r="C20" s="79"/>
+      <c r="D20" s="55"/>
+      <c r="E20" s="46"/>
+      <c r="F20" s="57"/>
+      <c r="G20" s="53"/>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A21" s="49"/>
+      <c r="B21" s="50"/>
+      <c r="C21" s="50"/>
+      <c r="D21" s="50"/>
+      <c r="E21" s="50"/>
+      <c r="F21" s="50"/>
+      <c r="G21" s="50"/>
+    </row>
+    <row r="22" spans="1:7" ht="56.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="78"/>
+      <c r="B22" s="79"/>
+      <c r="C22" s="55"/>
+      <c r="D22" s="55"/>
+      <c r="E22" s="56"/>
+      <c r="F22" s="57"/>
+      <c r="G22" s="53"/>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A23" s="49"/>
+      <c r="B23" s="50"/>
+      <c r="C23" s="50"/>
+      <c r="D23" s="50"/>
+      <c r="E23" s="50"/>
+      <c r="F23" s="50"/>
+      <c r="G23" s="50"/>
+    </row>
+    <row r="24" spans="1:7" ht="69" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="78"/>
+      <c r="B24" s="79"/>
+      <c r="C24" s="79"/>
+      <c r="D24" s="55"/>
+      <c r="E24" s="46"/>
+      <c r="F24" s="47"/>
+      <c r="G24" s="53"/>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A25" s="49"/>
+      <c r="B25" s="50"/>
+      <c r="C25" s="50"/>
+      <c r="D25" s="50"/>
+      <c r="E25" s="50"/>
+      <c r="F25" s="50"/>
+      <c r="G25" s="50"/>
+    </row>
+    <row r="26" spans="1:7" ht="58.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="78"/>
+      <c r="B26" s="79"/>
+      <c r="C26" s="79"/>
+      <c r="D26" s="55"/>
+      <c r="E26" s="46"/>
+      <c r="F26" s="47"/>
+      <c r="G26" s="53"/>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A27" s="49"/>
+      <c r="B27" s="50"/>
+      <c r="C27" s="50"/>
+      <c r="D27" s="50"/>
+      <c r="E27" s="50"/>
+      <c r="F27" s="50"/>
+      <c r="G27" s="50"/>
+    </row>
+    <row r="28" spans="1:7" ht="54" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="78"/>
+      <c r="B28" s="79"/>
+      <c r="C28" s="79"/>
+      <c r="D28" s="55"/>
+      <c r="E28" s="46"/>
+      <c r="F28" s="47"/>
+      <c r="G28" s="53"/>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A29" s="49"/>
+      <c r="B29" s="50"/>
+      <c r="C29" s="50"/>
+      <c r="D29" s="50"/>
+      <c r="E29" s="50"/>
+      <c r="F29" s="50"/>
+      <c r="G29" s="50"/>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A30" s="78"/>
+      <c r="B30" s="55"/>
+      <c r="C30" s="55"/>
+      <c r="D30" s="55"/>
+      <c r="E30" s="56"/>
+      <c r="F30" s="57"/>
+      <c r="G30" s="58"/>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A31" s="49"/>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A32" s="78"/>
+      <c r="B32" s="55"/>
+      <c r="C32" s="55"/>
+      <c r="D32" s="55"/>
+      <c r="E32" s="56"/>
+      <c r="F32" s="57"/>
+      <c r="G32" s="58"/>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A33" s="49"/>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A34" s="78"/>
+      <c r="B34" s="55"/>
+      <c r="C34" s="55"/>
+      <c r="D34" s="55"/>
+      <c r="E34" s="56"/>
+      <c r="F34" s="57"/>
+      <c r="G34" s="58"/>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A35" s="49"/>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A36" s="78"/>
+      <c r="B36" s="55"/>
+      <c r="C36" s="55"/>
+      <c r="D36" s="55"/>
+      <c r="E36" s="56"/>
+      <c r="F36" s="57"/>
+      <c r="G36" s="58"/>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A37" s="49"/>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A38" s="78"/>
+      <c r="B38" s="55"/>
+      <c r="C38" s="55"/>
+      <c r="D38" s="55"/>
+      <c r="E38" s="56"/>
+      <c r="F38" s="57"/>
+      <c r="G38" s="58"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B3:D3"/>
+  </mergeCells>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
versão congelada dos testes
</commit_message>
<xml_diff>
--- a/testes/cmproject_test_case.xlsx
+++ b/testes/cmproject_test_case.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="851" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="851" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Capa" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="386" uniqueCount="203">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="400" uniqueCount="215">
   <si>
     <t>Projeto de Teste</t>
   </si>
@@ -642,6 +642,42 @@
   </si>
   <si>
     <t>Mapa exibindo corretamente a localização da locadora de veículos</t>
+  </si>
+  <si>
+    <t>Ct-d003</t>
+  </si>
+  <si>
+    <t>Cadastrar com preço promocional</t>
+  </si>
+  <si>
+    <t>Ter login para acessar ações administrativas</t>
+  </si>
+  <si>
+    <t>Logar no sistema, acessar ações administrativas, clicar em cadastrar veículo, preecher os dados de entrada inserindo os dois preços.</t>
+  </si>
+  <si>
+    <t>Cadastro realizado com sucesso, e exibir na lista de nossos veículos com o valor promocional</t>
+  </si>
+  <si>
+    <t>dados solicitados no formulário inserindo o valor do preço promocional</t>
+  </si>
+  <si>
+    <t>Veículo cadastrado e listado como valor promocional</t>
+  </si>
+  <si>
+    <t>Ct-I002</t>
+  </si>
+  <si>
+    <t>Encontrar locadora a partir da tela de comprovanto</t>
+  </si>
+  <si>
+    <t>Ter alugado um veículo e estar na pagina de comprovante de aluguel</t>
+  </si>
+  <si>
+    <t>Clicar no botão de Localizar locadora</t>
+  </si>
+  <si>
+    <t>Pagina com o a localização da locadora exibida na tela</t>
   </si>
 </sst>
 </file>
@@ -726,7 +762,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="15">
+  <fills count="16">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -809,6 +845,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FF00B050"/>
         <bgColor rgb="FF993300"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor rgb="FFDCE6F2"/>
       </patternFill>
     </fill>
   </fills>
@@ -1023,7 +1065,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="89">
+  <cellXfs count="90">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1218,6 +1260,9 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="14" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1242,7 +1287,7 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="14" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="15" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1748,11 +1793,11 @@
       <c r="B13" s="4"/>
       <c r="C13" s="5"/>
       <c r="D13" s="10"/>
-      <c r="E13" s="80" t="s">
+      <c r="E13" s="81" t="s">
         <v>0</v>
       </c>
-      <c r="F13" s="80"/>
-      <c r="G13" s="80"/>
+      <c r="F13" s="81"/>
+      <c r="G13" s="81"/>
       <c r="H13" s="11"/>
       <c r="I13" s="5"/>
       <c r="J13" s="6"/>
@@ -1761,9 +1806,9 @@
       <c r="B14" s="4"/>
       <c r="C14" s="5"/>
       <c r="D14" s="10"/>
-      <c r="E14" s="80"/>
-      <c r="F14" s="80"/>
-      <c r="G14" s="80"/>
+      <c r="E14" s="81"/>
+      <c r="F14" s="81"/>
+      <c r="G14" s="81"/>
       <c r="H14" s="11"/>
       <c r="I14" s="5"/>
       <c r="J14" s="6"/>
@@ -1783,11 +1828,11 @@
       <c r="B16" s="4"/>
       <c r="C16" s="5"/>
       <c r="D16" s="10"/>
-      <c r="E16" s="81" t="s">
+      <c r="E16" s="82" t="s">
         <v>1</v>
       </c>
-      <c r="F16" s="81"/>
-      <c r="G16" s="81"/>
+      <c r="F16" s="82"/>
+      <c r="G16" s="82"/>
       <c r="H16" s="11"/>
       <c r="I16" s="5"/>
       <c r="J16" s="6"/>
@@ -1796,9 +1841,9 @@
       <c r="B17" s="4"/>
       <c r="C17" s="5"/>
       <c r="D17" s="10"/>
-      <c r="E17" s="81"/>
-      <c r="F17" s="81"/>
-      <c r="G17" s="81"/>
+      <c r="E17" s="82"/>
+      <c r="F17" s="82"/>
+      <c r="G17" s="82"/>
       <c r="H17" s="11"/>
       <c r="I17" s="5"/>
       <c r="J17" s="6"/>
@@ -1844,11 +1889,11 @@
       <c r="B21" s="4"/>
       <c r="C21" s="5"/>
       <c r="D21" s="10"/>
-      <c r="E21" s="82" t="s">
+      <c r="E21" s="83" t="s">
         <v>4</v>
       </c>
-      <c r="F21" s="82"/>
-      <c r="G21" s="82"/>
+      <c r="F21" s="83"/>
+      <c r="G21" s="83"/>
       <c r="H21" s="11"/>
       <c r="I21" s="5"/>
       <c r="J21" s="6"/>
@@ -1857,11 +1902,11 @@
       <c r="B22" s="4"/>
       <c r="C22" s="5"/>
       <c r="D22" s="10"/>
-      <c r="E22" s="82" t="s">
+      <c r="E22" s="83" t="s">
         <v>5</v>
       </c>
-      <c r="F22" s="82"/>
-      <c r="G22" s="82"/>
+      <c r="F22" s="83"/>
+      <c r="G22" s="83"/>
       <c r="H22" s="11"/>
       <c r="I22" s="5"/>
       <c r="J22" s="6"/>
@@ -1870,9 +1915,9 @@
       <c r="B23" s="4"/>
       <c r="C23" s="5"/>
       <c r="D23" s="10"/>
-      <c r="E23" s="83"/>
-      <c r="F23" s="83"/>
-      <c r="G23" s="83"/>
+      <c r="E23" s="84"/>
+      <c r="F23" s="84"/>
+      <c r="G23" s="84"/>
       <c r="H23" s="11"/>
       <c r="I23" s="5"/>
       <c r="J23" s="6"/>
@@ -2044,8 +2089,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G76"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2100,11 +2145,11 @@
       <c r="A3" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="84" t="s">
+      <c r="B3" s="85" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="84"/>
-      <c r="D3" s="84"/>
+      <c r="C3" s="85"/>
+      <c r="D3" s="85"/>
       <c r="E3" s="34"/>
       <c r="F3" s="35"/>
       <c r="G3" s="33"/>
@@ -2156,7 +2201,7 @@
       <c r="F6" s="47" t="s">
         <v>183</v>
       </c>
-      <c r="G6" s="88" t="s">
+      <c r="G6" s="80" t="s">
         <v>182</v>
       </c>
     </row>
@@ -2220,7 +2265,7 @@
       <c r="F10" s="47" t="s">
         <v>183</v>
       </c>
-      <c r="G10" s="88" t="s">
+      <c r="G10" s="80" t="s">
         <v>187</v>
       </c>
     </row>
@@ -2252,7 +2297,7 @@
       <c r="F12" s="47" t="s">
         <v>26</v>
       </c>
-      <c r="G12" s="88" t="s">
+      <c r="G12" s="80" t="s">
         <v>188</v>
       </c>
     </row>
@@ -2827,7 +2872,7 @@
   <dimension ref="A1:G38"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F10" sqref="A1:XFD1048576"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2882,11 +2927,11 @@
       <c r="A3" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="84" t="s">
+      <c r="B3" s="85" t="s">
         <v>63</v>
       </c>
-      <c r="C3" s="84"/>
-      <c r="D3" s="84"/>
+      <c r="C3" s="85"/>
+      <c r="D3" s="85"/>
       <c r="E3" s="34"/>
       <c r="F3" s="35"/>
       <c r="G3" s="33"/>
@@ -3307,11 +3352,11 @@
       <c r="A3" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="85" t="s">
+      <c r="B3" s="86" t="s">
         <v>78</v>
       </c>
-      <c r="C3" s="85"/>
-      <c r="D3" s="85"/>
+      <c r="C3" s="86"/>
+      <c r="D3" s="86"/>
       <c r="E3" s="34"/>
       <c r="F3" s="35"/>
       <c r="G3" s="66"/>
@@ -3724,11 +3769,11 @@
       <c r="A3" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="86" t="s">
+      <c r="B3" s="87" t="s">
         <v>102</v>
       </c>
-      <c r="C3" s="86"/>
-      <c r="D3" s="86"/>
+      <c r="C3" s="87"/>
+      <c r="D3" s="87"/>
       <c r="E3" s="34"/>
       <c r="F3" s="35"/>
       <c r="G3" s="66"/>
@@ -4117,8 +4162,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G56"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView topLeftCell="A8" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4173,11 +4218,11 @@
       <c r="A3" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="87" t="s">
+      <c r="B3" s="88" t="s">
         <v>102</v>
       </c>
-      <c r="C3" s="87"/>
-      <c r="D3" s="87"/>
+      <c r="C3" s="88"/>
+      <c r="D3" s="88"/>
       <c r="E3" s="34"/>
       <c r="F3" s="35"/>
       <c r="G3" s="66"/>
@@ -4370,14 +4415,28 @@
       <c r="F15" s="50"/>
       <c r="G15" s="68"/>
     </row>
-    <row r="16" spans="1:7" ht="47.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="44"/>
-      <c r="B16" s="45"/>
-      <c r="C16" s="45"/>
-      <c r="D16" s="45"/>
-      <c r="E16" s="46"/>
-      <c r="F16" s="52"/>
-      <c r="G16" s="69"/>
+    <row r="16" spans="1:7" ht="63.75" x14ac:dyDescent="0.2">
+      <c r="A16" s="44" t="s">
+        <v>203</v>
+      </c>
+      <c r="B16" s="45" t="s">
+        <v>204</v>
+      </c>
+      <c r="C16" s="45" t="s">
+        <v>205</v>
+      </c>
+      <c r="D16" s="45" t="s">
+        <v>206</v>
+      </c>
+      <c r="E16" s="46" t="s">
+        <v>207</v>
+      </c>
+      <c r="F16" s="52" t="s">
+        <v>208</v>
+      </c>
+      <c r="G16" s="89" t="s">
+        <v>209</v>
+      </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" s="54"/>
@@ -4722,8 +4781,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G38"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4777,11 +4836,11 @@
       <c r="A3" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="84" t="s">
+      <c r="B3" s="85" t="s">
         <v>191</v>
       </c>
-      <c r="C3" s="84"/>
-      <c r="D3" s="84"/>
+      <c r="C3" s="85"/>
+      <c r="D3" s="85"/>
       <c r="E3" s="34"/>
       <c r="F3" s="35"/>
       <c r="G3" s="33"/>
@@ -4846,14 +4905,28 @@
       <c r="F7" s="50"/>
       <c r="G7" s="50"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A8" s="78"/>
-      <c r="B8" s="79"/>
-      <c r="C8" s="78"/>
-      <c r="D8" s="79"/>
-      <c r="E8" s="46"/>
-      <c r="F8" s="47"/>
-      <c r="G8" s="58"/>
+    <row r="8" spans="1:7" ht="63.75" x14ac:dyDescent="0.2">
+      <c r="A8" s="78" t="s">
+        <v>210</v>
+      </c>
+      <c r="B8" s="79" t="s">
+        <v>211</v>
+      </c>
+      <c r="C8" s="78" t="s">
+        <v>212</v>
+      </c>
+      <c r="D8" s="79" t="s">
+        <v>213</v>
+      </c>
+      <c r="E8" s="46" t="s">
+        <v>214</v>
+      </c>
+      <c r="F8" s="47" t="s">
+        <v>26</v>
+      </c>
+      <c r="G8" s="75" t="s">
+        <v>202</v>
+      </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" s="54"/>

</xml_diff>